<commit_message>
There were a bunch of dates that were supposed to be in 2019 that were mistakenly dated 2020
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="440" windowWidth="24000" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces Eaten" sheetId="1" r:id="rId1"/>
@@ -963,8 +963,8 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A584" sqref="A584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="3">
-        <v>43472</v>
+        <v>43107</v>
       </c>
       <c r="B22" s="1">
         <v>7</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="63" spans="1:14" ht="15.75" customHeight="1">
       <c r="A63" s="3">
-        <v>42816</v>
+        <v>43181</v>
       </c>
       <c r="B63" s="1">
         <v>9</v>
@@ -3924,7 +3924,7 @@
     </row>
     <row r="76" spans="1:14" ht="15.75" customHeight="1">
       <c r="A76" s="3">
-        <v>43935</v>
+        <v>43204</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -7389,7 +7389,7 @@
     </row>
     <row r="165" spans="1:14" ht="15.75" customHeight="1">
       <c r="A165" s="3">
-        <v>43724</v>
+        <v>43359</v>
       </c>
       <c r="B165" s="1">
         <v>1</v>
@@ -8325,7 +8325,7 @@
     </row>
     <row r="189" spans="1:14" ht="15.75" customHeight="1">
       <c r="A189" s="3">
-        <v>43766</v>
+        <v>43401</v>
       </c>
       <c r="B189" s="1">
         <v>3</v>
@@ -8637,7 +8637,7 @@
     </row>
     <row r="197" spans="1:14" ht="15.75" customHeight="1">
       <c r="A197" s="3">
-        <v>43780</v>
+        <v>43415</v>
       </c>
       <c r="B197" s="1">
         <v>3</v>
@@ -12105,7 +12105,7 @@
     </row>
     <row r="286" spans="1:14" ht="15.75" customHeight="1">
       <c r="A286" s="3">
-        <v>43210</v>
+        <v>43575</v>
       </c>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
@@ -12996,7 +12996,7 @@
     </row>
     <row r="309" spans="1:14" ht="15.75" customHeight="1">
       <c r="A309" s="5">
-        <v>43981</v>
+        <v>43615</v>
       </c>
       <c r="B309" s="4">
         <v>7</v>
@@ -13041,7 +13041,7 @@
     </row>
     <row r="310" spans="1:14" ht="15.75" customHeight="1">
       <c r="A310" s="5">
-        <v>43983</v>
+        <v>43617</v>
       </c>
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
@@ -13072,7 +13072,7 @@
     </row>
     <row r="311" spans="1:14" ht="15.75" customHeight="1">
       <c r="A311" s="5">
-        <v>43984</v>
+        <v>43618</v>
       </c>
       <c r="B311" s="4">
         <v>7</v>
@@ -13107,7 +13107,7 @@
     </row>
     <row r="312" spans="1:14" ht="15.75" customHeight="1">
       <c r="A312" s="5">
-        <v>43986</v>
+        <v>43620</v>
       </c>
       <c r="B312" s="4">
         <v>2</v>
@@ -13152,7 +13152,7 @@
     </row>
     <row r="313" spans="1:14" ht="15.75" customHeight="1">
       <c r="A313" s="5">
-        <v>43988</v>
+        <v>43622</v>
       </c>
       <c r="B313" s="4">
         <v>8</v>
@@ -13197,7 +13197,7 @@
     </row>
     <row r="314" spans="1:14" ht="15.75" customHeight="1">
       <c r="A314" s="5">
-        <v>43990</v>
+        <v>43624</v>
       </c>
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
@@ -13228,7 +13228,7 @@
     </row>
     <row r="315" spans="1:14" ht="15.75" customHeight="1">
       <c r="A315" s="5">
-        <v>43991</v>
+        <v>43625</v>
       </c>
       <c r="B315" s="4">
         <v>4</v>
@@ -13263,7 +13263,7 @@
     </row>
     <row r="316" spans="1:14" ht="15.75" customHeight="1">
       <c r="A316" s="5">
-        <v>43993</v>
+        <v>43627</v>
       </c>
       <c r="B316" s="4">
         <v>0</v>
@@ -13308,7 +13308,7 @@
     </row>
     <row r="317" spans="1:14" ht="15.75" customHeight="1">
       <c r="A317" s="5">
-        <v>43995</v>
+        <v>43629</v>
       </c>
       <c r="B317" s="4">
         <v>6</v>
@@ -13353,7 +13353,7 @@
     </row>
     <row r="318" spans="1:14" ht="15.75" customHeight="1">
       <c r="A318" s="5">
-        <v>43997</v>
+        <v>43631</v>
       </c>
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
@@ -13384,7 +13384,7 @@
     </row>
     <row r="319" spans="1:14" ht="15.75" customHeight="1">
       <c r="A319" s="5">
-        <v>43998</v>
+        <v>43632</v>
       </c>
       <c r="B319" s="4">
         <v>3</v>
@@ -13419,7 +13419,7 @@
     </row>
     <row r="320" spans="1:14" ht="15.75" customHeight="1">
       <c r="A320" s="5">
-        <v>44000</v>
+        <v>43634</v>
       </c>
       <c r="B320" s="4">
         <v>0</v>
@@ -13464,7 +13464,7 @@
     </row>
     <row r="321" spans="1:14" ht="15.75" customHeight="1">
       <c r="A321" s="5">
-        <v>44002</v>
+        <v>43636</v>
       </c>
       <c r="B321" s="4">
         <v>3</v>
@@ -13509,7 +13509,7 @@
     </row>
     <row r="322" spans="1:14" ht="15.75" customHeight="1">
       <c r="A322" s="5">
-        <v>44004</v>
+        <v>43638</v>
       </c>
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
@@ -13540,7 +13540,7 @@
     </row>
     <row r="323" spans="1:14" ht="15.75" customHeight="1">
       <c r="A323" s="5">
-        <v>44005</v>
+        <v>43639</v>
       </c>
       <c r="B323" s="4">
         <v>14</v>
@@ -13575,7 +13575,7 @@
     </row>
     <row r="324" spans="1:14" ht="15.75" customHeight="1">
       <c r="A324" s="5">
-        <v>44007</v>
+        <v>43641</v>
       </c>
       <c r="B324" s="4">
         <v>7</v>
@@ -13620,7 +13620,7 @@
     </row>
     <row r="325" spans="1:14" ht="15.75" customHeight="1">
       <c r="A325" s="5">
-        <v>44009</v>
+        <v>43643</v>
       </c>
       <c r="B325" s="4">
         <v>6</v>
@@ -13665,7 +13665,7 @@
     </row>
     <row r="326" spans="1:14" ht="15.75" customHeight="1">
       <c r="A326" s="5">
-        <v>44011</v>
+        <v>43645</v>
       </c>
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
@@ -13696,7 +13696,7 @@
     </row>
     <row r="327" spans="1:14" ht="15.75" customHeight="1">
       <c r="A327" s="5">
-        <v>44012</v>
+        <v>43646</v>
       </c>
       <c r="B327" s="4">
         <v>1</v>
@@ -13731,7 +13731,7 @@
     </row>
     <row r="328" spans="1:14" ht="15.75" customHeight="1">
       <c r="A328" s="5">
-        <v>44014</v>
+        <v>43648</v>
       </c>
       <c r="B328" s="4">
         <v>7</v>
@@ -13776,7 +13776,7 @@
     </row>
     <row r="329" spans="1:14" ht="15.75" customHeight="1">
       <c r="A329" s="5">
-        <v>44016</v>
+        <v>43650</v>
       </c>
       <c r="B329" s="4">
         <v>5</v>
@@ -13821,7 +13821,7 @@
     </row>
     <row r="330" spans="1:14" ht="15.75" customHeight="1">
       <c r="A330" s="5">
-        <v>44018</v>
+        <v>43652</v>
       </c>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -13852,7 +13852,7 @@
     </row>
     <row r="331" spans="1:14" ht="15.75" customHeight="1">
       <c r="A331" s="5">
-        <v>43989</v>
+        <v>43623</v>
       </c>
       <c r="B331" s="4">
         <v>3</v>
@@ -13887,7 +13887,7 @@
     </row>
     <row r="332" spans="1:14" ht="15.75" customHeight="1">
       <c r="A332" s="5">
-        <v>43991</v>
+        <v>43625</v>
       </c>
       <c r="B332" s="4">
         <v>8</v>
@@ -13932,7 +13932,7 @@
     </row>
     <row r="333" spans="1:14" ht="15.75" customHeight="1">
       <c r="A333" s="5">
-        <v>44023</v>
+        <v>43657</v>
       </c>
       <c r="B333" s="4">
         <v>2</v>
@@ -13977,7 +13977,7 @@
     </row>
     <row r="334" spans="1:14" ht="15.75" customHeight="1">
       <c r="A334" s="5">
-        <v>44025</v>
+        <v>43659</v>
       </c>
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
@@ -14008,7 +14008,7 @@
     </row>
     <row r="335" spans="1:14" ht="15.75" customHeight="1">
       <c r="A335" s="5">
-        <v>44026</v>
+        <v>43660</v>
       </c>
       <c r="B335" s="4">
         <v>4</v>
@@ -14043,7 +14043,7 @@
     </row>
     <row r="336" spans="1:14" ht="15.75" customHeight="1">
       <c r="A336" s="5">
-        <v>44028</v>
+        <v>43662</v>
       </c>
       <c r="B336" s="4">
         <v>6</v>
@@ -14088,7 +14088,7 @@
     </row>
     <row r="337" spans="1:14" ht="15.75" customHeight="1">
       <c r="A337" s="5">
-        <v>44030</v>
+        <v>43664</v>
       </c>
       <c r="B337" s="4">
         <v>1</v>
@@ -14133,7 +14133,7 @@
     </row>
     <row r="338" spans="1:14" ht="15.75" customHeight="1">
       <c r="A338" s="5">
-        <v>44032</v>
+        <v>43666</v>
       </c>
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
@@ -14164,7 +14164,7 @@
     </row>
     <row r="339" spans="1:14" ht="15.75" customHeight="1">
       <c r="A339" s="5">
-        <v>44033</v>
+        <v>43667</v>
       </c>
       <c r="B339" s="4">
         <v>3</v>
@@ -14199,7 +14199,7 @@
     </row>
     <row r="340" spans="1:14" ht="15.75" customHeight="1">
       <c r="A340" s="5">
-        <v>44035</v>
+        <v>43669</v>
       </c>
       <c r="B340" s="4">
         <v>0</v>
@@ -14244,7 +14244,7 @@
     </row>
     <row r="341" spans="1:14" ht="15.75" customHeight="1">
       <c r="A341" s="5">
-        <v>44037</v>
+        <v>43671</v>
       </c>
       <c r="B341" s="4">
         <v>4</v>
@@ -14289,7 +14289,7 @@
     </row>
     <row r="342" spans="1:14" ht="15.75" customHeight="1">
       <c r="A342" s="5">
-        <v>44039</v>
+        <v>43673</v>
       </c>
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
@@ -14320,7 +14320,7 @@
     </row>
     <row r="343" spans="1:14" ht="15.75" customHeight="1">
       <c r="A343" s="5">
-        <v>44040</v>
+        <v>43674</v>
       </c>
       <c r="B343" s="4">
         <v>3</v>
@@ -14355,7 +14355,7 @@
     </row>
     <row r="344" spans="1:14" ht="15.75" customHeight="1">
       <c r="A344" s="5">
-        <v>44042</v>
+        <v>43676</v>
       </c>
       <c r="B344" s="4">
         <v>5</v>
@@ -14400,7 +14400,7 @@
     </row>
     <row r="345" spans="1:14" ht="15.75" customHeight="1">
       <c r="A345" s="5">
-        <v>44044</v>
+        <v>43678</v>
       </c>
       <c r="B345" s="4">
         <v>1</v>
@@ -14445,7 +14445,7 @@
     </row>
     <row r="346" spans="1:14" ht="15.75" customHeight="1">
       <c r="A346" s="5">
-        <v>44046</v>
+        <v>43680</v>
       </c>
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
@@ -14476,7 +14476,7 @@
     </row>
     <row r="347" spans="1:14" ht="15.75" customHeight="1">
       <c r="A347" s="5">
-        <v>44047</v>
+        <v>43681</v>
       </c>
       <c r="B347" s="4">
         <v>9</v>
@@ -14511,7 +14511,7 @@
     </row>
     <row r="348" spans="1:14" ht="15.75" customHeight="1">
       <c r="A348" s="5">
-        <v>44049</v>
+        <v>43683</v>
       </c>
       <c r="B348" s="4">
         <v>0</v>
@@ -14556,7 +14556,7 @@
     </row>
     <row r="349" spans="1:14" ht="15.75" customHeight="1">
       <c r="A349" s="5">
-        <v>44051</v>
+        <v>43685</v>
       </c>
       <c r="B349" s="4">
         <v>7</v>
@@ -14601,7 +14601,7 @@
     </row>
     <row r="350" spans="1:14" ht="15.75" customHeight="1">
       <c r="A350" s="5">
-        <v>44053</v>
+        <v>43687</v>
       </c>
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
@@ -14632,7 +14632,7 @@
     </row>
     <row r="351" spans="1:14" ht="15.75" customHeight="1">
       <c r="A351" s="5">
-        <v>44054</v>
+        <v>43688</v>
       </c>
       <c r="B351" s="4">
         <v>5</v>
@@ -14667,7 +14667,7 @@
     </row>
     <row r="352" spans="1:14" ht="15.75" customHeight="1">
       <c r="A352" s="5">
-        <v>44056</v>
+        <v>43690</v>
       </c>
       <c r="B352" s="4">
         <v>2</v>
@@ -14712,7 +14712,7 @@
     </row>
     <row r="353" spans="1:14" ht="15.75" customHeight="1">
       <c r="A353" s="5">
-        <v>44058</v>
+        <v>43692</v>
       </c>
       <c r="B353" s="4">
         <v>2</v>
@@ -14757,7 +14757,7 @@
     </row>
     <row r="354" spans="1:14" ht="15.75" customHeight="1">
       <c r="A354" s="5">
-        <v>44060</v>
+        <v>43694</v>
       </c>
       <c r="B354" s="1"/>
       <c r="C354" s="1"/>
@@ -14788,7 +14788,7 @@
     </row>
     <row r="355" spans="1:14" ht="15.75" customHeight="1">
       <c r="A355" s="5">
-        <v>44061</v>
+        <v>43695</v>
       </c>
       <c r="B355" s="4">
         <v>3</v>
@@ -14823,7 +14823,7 @@
     </row>
     <row r="356" spans="1:14" ht="15.75" customHeight="1">
       <c r="A356" s="5">
-        <v>44063</v>
+        <v>43697</v>
       </c>
       <c r="B356" s="4">
         <v>0</v>
@@ -14868,7 +14868,7 @@
     </row>
     <row r="357" spans="1:14" ht="15.75" customHeight="1">
       <c r="A357" s="5">
-        <v>44065</v>
+        <v>43699</v>
       </c>
       <c r="B357" s="4">
         <v>7</v>
@@ -14913,7 +14913,7 @@
     </row>
     <row r="358" spans="1:14" ht="15.75" customHeight="1">
       <c r="A358" s="5">
-        <v>44067</v>
+        <v>43701</v>
       </c>
       <c r="B358" s="1"/>
       <c r="C358" s="1"/>
@@ -14944,7 +14944,7 @@
     </row>
     <row r="359" spans="1:14" ht="15.75" customHeight="1">
       <c r="A359" s="5">
-        <v>44068</v>
+        <v>43702</v>
       </c>
       <c r="B359" s="4">
         <v>5</v>
@@ -14979,7 +14979,7 @@
     </row>
     <row r="360" spans="1:14" ht="15.75" customHeight="1">
       <c r="A360" s="5">
-        <v>44070</v>
+        <v>43704</v>
       </c>
       <c r="B360" s="4">
         <v>6</v>
@@ -15024,7 +15024,7 @@
     </row>
     <row r="361" spans="1:14" ht="15.75" customHeight="1">
       <c r="A361" s="5">
-        <v>44072</v>
+        <v>43706</v>
       </c>
       <c r="B361" s="4">
         <v>2</v>
@@ -15069,7 +15069,7 @@
     </row>
     <row r="362" spans="1:14" ht="15.75" customHeight="1">
       <c r="A362" s="5">
-        <v>44074</v>
+        <v>43708</v>
       </c>
       <c r="B362" s="1"/>
       <c r="C362" s="1"/>
@@ -15100,7 +15100,7 @@
     </row>
     <row r="363" spans="1:14" ht="15.75" customHeight="1">
       <c r="A363" s="5">
-        <v>44075</v>
+        <v>43709</v>
       </c>
       <c r="B363" s="4">
         <v>9</v>
@@ -15135,7 +15135,7 @@
     </row>
     <row r="364" spans="1:14" ht="15.75" customHeight="1">
       <c r="A364" s="5">
-        <v>44077</v>
+        <v>43711</v>
       </c>
       <c r="B364" s="4">
         <v>2</v>
@@ -15180,7 +15180,7 @@
     </row>
     <row r="365" spans="1:14" ht="15.75" customHeight="1">
       <c r="A365" s="5">
-        <v>44079</v>
+        <v>43713</v>
       </c>
       <c r="B365" s="4">
         <v>4</v>
@@ -15225,7 +15225,7 @@
     </row>
     <row r="366" spans="1:14" ht="15.75" customHeight="1">
       <c r="A366" s="5">
-        <v>44081</v>
+        <v>43715</v>
       </c>
       <c r="B366" s="1"/>
       <c r="C366" s="1"/>
@@ -15256,7 +15256,7 @@
     </row>
     <row r="367" spans="1:14" ht="15.75" customHeight="1">
       <c r="A367" s="5">
-        <v>44082</v>
+        <v>43716</v>
       </c>
       <c r="B367" s="4">
         <v>4</v>
@@ -15291,7 +15291,7 @@
     </row>
     <row r="368" spans="1:14" ht="15.75" customHeight="1">
       <c r="A368" s="5">
-        <v>44084</v>
+        <v>43718</v>
       </c>
       <c r="B368" s="4">
         <v>3</v>
@@ -15336,7 +15336,7 @@
     </row>
     <row r="369" spans="1:14" ht="15.75" customHeight="1">
       <c r="A369" s="5">
-        <v>44086</v>
+        <v>43720</v>
       </c>
       <c r="B369" s="4">
         <v>2</v>
@@ -15381,7 +15381,7 @@
     </row>
     <row r="370" spans="1:14" ht="15.75" customHeight="1">
       <c r="A370" s="5">
-        <v>44088</v>
+        <v>43722</v>
       </c>
       <c r="B370" s="1"/>
       <c r="C370" s="1"/>
@@ -15412,7 +15412,7 @@
     </row>
     <row r="371" spans="1:14" ht="15.75" customHeight="1">
       <c r="A371" s="5">
-        <v>44089</v>
+        <v>43723</v>
       </c>
       <c r="B371" s="4">
         <v>1</v>
@@ -15447,7 +15447,7 @@
     </row>
     <row r="372" spans="1:14" ht="15.75" customHeight="1">
       <c r="A372" s="5">
-        <v>44091</v>
+        <v>43725</v>
       </c>
       <c r="B372" s="4">
         <v>2</v>
@@ -15492,7 +15492,7 @@
     </row>
     <row r="373" spans="1:14" ht="15.75" customHeight="1">
       <c r="A373" s="5">
-        <v>44092</v>
+        <v>43726</v>
       </c>
       <c r="B373" s="4">
         <v>7</v>
@@ -15537,7 +15537,7 @@
     </row>
     <row r="374" spans="1:14" ht="15.75" customHeight="1">
       <c r="A374" s="5">
-        <v>44095</v>
+        <v>43729</v>
       </c>
       <c r="B374" s="4">
         <v>1</v>
@@ -15570,7 +15570,7 @@
     </row>
     <row r="375" spans="1:14" ht="15.75" customHeight="1">
       <c r="A375" s="5">
-        <v>44096</v>
+        <v>43730</v>
       </c>
       <c r="B375" s="4">
         <v>4</v>
@@ -15605,7 +15605,7 @@
     </row>
     <row r="376" spans="1:14" ht="15.75" customHeight="1">
       <c r="A376" s="5">
-        <v>44098</v>
+        <v>43732</v>
       </c>
       <c r="B376" s="4">
         <v>4</v>
@@ -15650,7 +15650,7 @@
     </row>
     <row r="377" spans="1:14" ht="15.75" customHeight="1">
       <c r="A377" s="5">
-        <v>44100</v>
+        <v>43734</v>
       </c>
       <c r="B377" s="4">
         <v>4</v>
@@ -15695,7 +15695,7 @@
     </row>
     <row r="378" spans="1:14" ht="15.75" customHeight="1">
       <c r="A378" s="5">
-        <v>44102</v>
+        <v>43736</v>
       </c>
       <c r="B378" s="1"/>
       <c r="C378" s="1"/>
@@ -15726,7 +15726,7 @@
     </row>
     <row r="379" spans="1:14" ht="15.75" customHeight="1">
       <c r="A379" s="5">
-        <v>44103</v>
+        <v>43737</v>
       </c>
       <c r="B379" s="4">
         <v>9</v>
@@ -15761,7 +15761,7 @@
     </row>
     <row r="380" spans="1:14" ht="15.75" customHeight="1">
       <c r="A380" s="5">
-        <v>44105</v>
+        <v>43739</v>
       </c>
       <c r="B380" s="4">
         <v>1</v>
@@ -15806,7 +15806,7 @@
     </row>
     <row r="381" spans="1:14" ht="15.75" customHeight="1">
       <c r="A381" s="5">
-        <v>44107</v>
+        <v>43741</v>
       </c>
       <c r="B381" s="4">
         <v>4</v>
@@ -15851,7 +15851,7 @@
     </row>
     <row r="382" spans="1:14" ht="15.75" customHeight="1">
       <c r="A382" s="5">
-        <v>44109</v>
+        <v>43743</v>
       </c>
       <c r="B382" s="1"/>
       <c r="C382" s="1"/>
@@ -15882,7 +15882,7 @@
     </row>
     <row r="383" spans="1:14" ht="15.75" customHeight="1">
       <c r="A383" s="5">
-        <v>44110</v>
+        <v>43744</v>
       </c>
       <c r="B383" s="4">
         <v>8</v>
@@ -15917,7 +15917,7 @@
     </row>
     <row r="384" spans="1:14" ht="15.75" customHeight="1">
       <c r="A384" s="5">
-        <v>44112</v>
+        <v>43746</v>
       </c>
       <c r="B384" s="4">
         <v>3</v>
@@ -15962,7 +15962,7 @@
     </row>
     <row r="385" spans="1:14" ht="15.75" customHeight="1">
       <c r="A385" s="5">
-        <v>44114</v>
+        <v>43748</v>
       </c>
       <c r="B385" s="4">
         <v>5</v>
@@ -16007,7 +16007,7 @@
     </row>
     <row r="386" spans="1:14" ht="15.75" customHeight="1">
       <c r="A386" s="5">
-        <v>44116</v>
+        <v>43750</v>
       </c>
       <c r="B386" s="1"/>
       <c r="C386" s="1"/>
@@ -16038,7 +16038,7 @@
     </row>
     <row r="387" spans="1:14" ht="15.75" customHeight="1">
       <c r="A387" s="5">
-        <v>44117</v>
+        <v>43751</v>
       </c>
       <c r="B387" s="4">
         <v>4</v>
@@ -16073,7 +16073,7 @@
     </row>
     <row r="388" spans="1:14" ht="15.75" customHeight="1">
       <c r="A388" s="5">
-        <v>44119</v>
+        <v>43753</v>
       </c>
       <c r="B388" s="4">
         <v>7</v>
@@ -16118,7 +16118,7 @@
     </row>
     <row r="389" spans="1:14" ht="15.75" customHeight="1">
       <c r="A389" s="5">
-        <v>44121</v>
+        <v>43755</v>
       </c>
       <c r="B389" s="4">
         <v>5</v>
@@ -16163,7 +16163,7 @@
     </row>
     <row r="390" spans="1:14" ht="15.75" customHeight="1">
       <c r="A390" s="5">
-        <v>44123</v>
+        <v>43757</v>
       </c>
       <c r="B390" s="1"/>
       <c r="C390" s="1"/>
@@ -16194,7 +16194,7 @@
     </row>
     <row r="391" spans="1:14" ht="15.75" customHeight="1">
       <c r="A391" s="5">
-        <v>44124</v>
+        <v>43758</v>
       </c>
       <c r="B391" s="4">
         <v>3</v>
@@ -16229,7 +16229,7 @@
     </row>
     <row r="392" spans="1:14" ht="15.75" customHeight="1">
       <c r="A392" s="5">
-        <v>44126</v>
+        <v>43760</v>
       </c>
       <c r="B392" s="4">
         <v>4</v>
@@ -16274,7 +16274,7 @@
     </row>
     <row r="393" spans="1:14" ht="15.75" customHeight="1">
       <c r="A393" s="5">
-        <v>44128</v>
+        <v>43762</v>
       </c>
       <c r="B393" s="4">
         <v>0</v>
@@ -16319,7 +16319,7 @@
     </row>
     <row r="394" spans="1:14" ht="15.75" customHeight="1">
       <c r="A394" s="5">
-        <v>44130</v>
+        <v>43764</v>
       </c>
       <c r="B394" s="1"/>
       <c r="C394" s="1"/>
@@ -16350,7 +16350,7 @@
     </row>
     <row r="395" spans="1:14" ht="15.75" customHeight="1">
       <c r="A395" s="5">
-        <v>44132</v>
+        <v>43766</v>
       </c>
       <c r="B395" s="4">
         <v>6</v>
@@ -16385,7 +16385,7 @@
     </row>
     <row r="396" spans="1:14" ht="15.75" customHeight="1">
       <c r="A396" s="5">
-        <v>44133</v>
+        <v>43767</v>
       </c>
       <c r="B396" s="4">
         <v>0</v>
@@ -16430,7 +16430,7 @@
     </row>
     <row r="397" spans="1:14" ht="15.75" customHeight="1">
       <c r="A397" s="5">
-        <v>44135</v>
+        <v>43769</v>
       </c>
       <c r="B397" s="4">
         <v>2</v>
@@ -16475,7 +16475,7 @@
     </row>
     <row r="398" spans="1:14" ht="15.75" customHeight="1">
       <c r="A398" s="5">
-        <v>44137</v>
+        <v>43771</v>
       </c>
       <c r="B398" s="1"/>
       <c r="C398" s="1"/>
@@ -16506,7 +16506,7 @@
     </row>
     <row r="399" spans="1:14" ht="15.75" customHeight="1">
       <c r="A399" s="5">
-        <v>44138</v>
+        <v>43772</v>
       </c>
       <c r="B399" s="4">
         <v>6</v>
@@ -16541,7 +16541,7 @@
     </row>
     <row r="400" spans="1:14" ht="15.75" customHeight="1">
       <c r="A400" s="5">
-        <v>44140</v>
+        <v>43774</v>
       </c>
       <c r="B400" s="4">
         <v>2</v>
@@ -16586,7 +16586,7 @@
     </row>
     <row r="401" spans="1:14" ht="15.75" customHeight="1">
       <c r="A401" s="5">
-        <v>44142</v>
+        <v>43776</v>
       </c>
       <c r="B401" s="4">
         <v>1</v>
@@ -16631,7 +16631,7 @@
     </row>
     <row r="402" spans="1:14" ht="15.75" customHeight="1">
       <c r="A402" s="5">
-        <v>44144</v>
+        <v>43778</v>
       </c>
       <c r="B402" s="1"/>
       <c r="C402" s="1"/>
@@ -16662,7 +16662,7 @@
     </row>
     <row r="403" spans="1:14" ht="15.75" customHeight="1">
       <c r="A403" s="5">
-        <v>44145</v>
+        <v>43779</v>
       </c>
       <c r="B403" s="4">
         <v>2</v>
@@ -16697,7 +16697,7 @@
     </row>
     <row r="404" spans="1:14" ht="15.75" customHeight="1">
       <c r="A404" s="5">
-        <v>44147</v>
+        <v>43781</v>
       </c>
       <c r="B404" s="4">
         <v>1</v>
@@ -16742,7 +16742,7 @@
     </row>
     <row r="405" spans="1:14" ht="15.75" customHeight="1">
       <c r="A405" s="5">
-        <v>44149</v>
+        <v>43783</v>
       </c>
       <c r="B405" s="4">
         <v>0</v>
@@ -16787,7 +16787,7 @@
     </row>
     <row r="406" spans="1:14" ht="15.75" customHeight="1">
       <c r="A406" s="5">
-        <v>44151</v>
+        <v>43785</v>
       </c>
       <c r="B406" s="1"/>
       <c r="C406" s="1"/>
@@ -16818,7 +16818,7 @@
     </row>
     <row r="407" spans="1:14" ht="15.75" customHeight="1">
       <c r="A407" s="5">
-        <v>44152</v>
+        <v>43786</v>
       </c>
       <c r="B407" s="4">
         <v>3</v>
@@ -16853,7 +16853,7 @@
     </row>
     <row r="408" spans="1:14" ht="15.75" customHeight="1">
       <c r="A408" s="5">
-        <v>44154</v>
+        <v>43788</v>
       </c>
       <c r="B408" s="4">
         <v>5</v>
@@ -16898,7 +16898,7 @@
     </row>
     <row r="409" spans="1:14" ht="15.75" customHeight="1">
       <c r="A409" s="5">
-        <v>44156</v>
+        <v>43790</v>
       </c>
       <c r="B409" s="4">
         <v>2</v>
@@ -16943,7 +16943,7 @@
     </row>
     <row r="410" spans="1:14" ht="15.75" customHeight="1">
       <c r="A410" s="5">
-        <v>44158</v>
+        <v>43792</v>
       </c>
       <c r="B410" s="1"/>
       <c r="C410" s="1"/>
@@ -16974,7 +16974,7 @@
     </row>
     <row r="411" spans="1:14" ht="15.75" customHeight="1">
       <c r="A411" s="5">
-        <v>44159</v>
+        <v>43793</v>
       </c>
       <c r="B411" s="4">
         <v>5</v>
@@ -17009,7 +17009,7 @@
     </row>
     <row r="412" spans="1:14" ht="15.75" customHeight="1">
       <c r="A412" s="5">
-        <v>44161</v>
+        <v>43795</v>
       </c>
       <c r="B412" s="4">
         <v>0</v>
@@ -17054,7 +17054,7 @@
     </row>
     <row r="413" spans="1:14" ht="15.75" customHeight="1">
       <c r="A413" s="5">
-        <v>44165</v>
+        <v>43799</v>
       </c>
       <c r="B413" s="1"/>
       <c r="C413" s="1"/>
@@ -17085,7 +17085,7 @@
     </row>
     <row r="414" spans="1:14" ht="15.75" customHeight="1">
       <c r="A414" s="5">
-        <v>44166</v>
+        <v>43800</v>
       </c>
       <c r="B414" s="4">
         <v>3</v>
@@ -17120,7 +17120,7 @@
     </row>
     <row r="415" spans="1:14" ht="15.75" customHeight="1">
       <c r="A415" s="5">
-        <v>44168</v>
+        <v>43802</v>
       </c>
       <c r="B415" s="4">
         <v>3</v>
@@ -17165,7 +17165,7 @@
     </row>
     <row r="416" spans="1:14" ht="15.75" customHeight="1">
       <c r="A416" s="5">
-        <v>44170</v>
+        <v>43804</v>
       </c>
       <c r="B416" s="4">
         <v>0</v>
@@ -17210,7 +17210,7 @@
     </row>
     <row r="417" spans="1:16" ht="15.75" customHeight="1">
       <c r="A417" s="5">
-        <v>44172</v>
+        <v>43806</v>
       </c>
       <c r="B417" s="4"/>
       <c r="C417" s="4"/>
@@ -17241,7 +17241,7 @@
     </row>
     <row r="418" spans="1:16" ht="15.75" customHeight="1">
       <c r="A418" s="5">
-        <v>44173</v>
+        <v>43807</v>
       </c>
       <c r="B418" s="4">
         <v>0</v>
@@ -17276,7 +17276,7 @@
     </row>
     <row r="419" spans="1:16" ht="15.75" customHeight="1">
       <c r="A419" s="5">
-        <v>44175</v>
+        <v>43809</v>
       </c>
       <c r="B419" s="4">
         <v>0</v>
@@ -17321,7 +17321,7 @@
     </row>
     <row r="420" spans="1:16" ht="15.75" customHeight="1">
       <c r="A420" s="5">
-        <v>44177</v>
+        <v>43811</v>
       </c>
       <c r="B420" s="4">
         <v>2</v>
@@ -17366,7 +17366,7 @@
     </row>
     <row r="421" spans="1:16" ht="15.75" customHeight="1">
       <c r="A421" s="5">
-        <v>44180</v>
+        <v>43814</v>
       </c>
       <c r="B421" s="1"/>
       <c r="C421" s="1"/>
@@ -17397,7 +17397,7 @@
     </row>
     <row r="422" spans="1:16" ht="15.75" customHeight="1">
       <c r="A422" s="5">
-        <v>44181</v>
+        <v>43815</v>
       </c>
       <c r="B422" s="4">
         <v>9</v>
@@ -17432,7 +17432,7 @@
     </row>
     <row r="423" spans="1:16" ht="15.75" customHeight="1">
       <c r="A423" s="5">
-        <v>44182</v>
+        <v>43816</v>
       </c>
       <c r="B423" s="4">
         <v>6</v>
@@ -17477,7 +17477,7 @@
     </row>
     <row r="424" spans="1:16" ht="15.75" customHeight="1">
       <c r="A424" s="5">
-        <v>44184</v>
+        <v>43818</v>
       </c>
       <c r="B424" s="4">
         <v>4</v>
@@ -17522,7 +17522,7 @@
     </row>
     <row r="425" spans="1:16" ht="15.75" customHeight="1">
       <c r="A425" s="5">
-        <v>44186</v>
+        <v>43820</v>
       </c>
       <c r="B425" s="1"/>
       <c r="C425" s="1"/>
@@ -17553,7 +17553,7 @@
     </row>
     <row r="426" spans="1:16" ht="15.75" customHeight="1">
       <c r="A426" s="5">
-        <v>44187</v>
+        <v>43821</v>
       </c>
       <c r="B426" s="4">
         <v>6</v>
@@ -17588,7 +17588,7 @@
     </row>
     <row r="427" spans="1:16" ht="15.75" customHeight="1">
       <c r="A427" s="5">
-        <v>44189</v>
+        <v>43823</v>
       </c>
       <c r="B427" s="4">
         <v>1</v>
@@ -17633,7 +17633,7 @@
     </row>
     <row r="428" spans="1:16" ht="15.75" customHeight="1">
       <c r="A428" s="5">
-        <v>44191</v>
+        <v>43825</v>
       </c>
       <c r="B428" s="4">
         <v>7</v>
@@ -17678,7 +17678,7 @@
     </row>
     <row r="429" spans="1:16" ht="15.75" customHeight="1">
       <c r="A429" s="5">
-        <v>44193</v>
+        <v>43827</v>
       </c>
       <c r="B429" s="1"/>
       <c r="C429" s="1"/>
@@ -17709,7 +17709,7 @@
     </row>
     <row r="430" spans="1:16" ht="15.75" customHeight="1">
       <c r="A430" s="5">
-        <v>44194</v>
+        <v>43828</v>
       </c>
       <c r="B430" s="4">
         <v>3</v>
@@ -17744,7 +17744,7 @@
     </row>
     <row r="431" spans="1:16" ht="15.75" customHeight="1">
       <c r="A431" s="5">
-        <v>44196</v>
+        <v>43830</v>
       </c>
       <c r="B431" s="4">
         <v>5</v>
@@ -22954,7 +22954,7 @@
       <c r="L563" s="1"/>
       <c r="M563" s="1"/>
       <c r="N563" s="7">
-        <f t="shared" ref="N563:N626" si="7">SUM(B563:M563)</f>
+        <f t="shared" ref="N563:N593" si="7">SUM(B563:M563)</f>
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
There were a couple more errors that I found in the drops excel sheet that I had to fix. I was also thinking about looking at how much they dropped over time using a line graph but I got stuck for now and I will try again later.
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/753f33f7ae04b4eb/Documents/Fall 2020/Stat 495R/final-project-danny_brady_michael/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A23E0199-357D-433A-818F-A13EF11BEF08}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06C0477E-4C39-458A-BFE4-0CE6FCC1535B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces Eaten" sheetId="1" r:id="rId1"/>
@@ -919,9 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A333" sqref="A333"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46243,9 +46243,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O593"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O584" sqref="O584"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -48170,7 +48170,7 @@
     </row>
     <row r="54" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>39512</v>
+        <v>43164</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -48503,7 +48503,7 @@
     </row>
     <row r="63" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>42816</v>
+        <v>43181</v>
       </c>
       <c r="B63">
         <v>0</v>

</xml_diff>

<commit_message>
There was a lot of the data that was incorrect. A lot of the dates for targets and drops datasets were in 2020 when they shouldn't have been. They are corrected and noted in the word document that I have made to note of the changes we have done.
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/753f33f7ae04b4eb/Documents/Fall 2020/Stat 495R/final-project-danny_brady_michael/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06C0477E-4C39-458A-BFE4-0CE6FCC1535B}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55C1D362-3F6B-40E7-85A7-B2CD78818E77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,8 +44,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={88BA8BB9-D010-4657-ACA8-10E27501E5A7}</author>
-    <author>tc={E312AADC-0ECB-428F-9DB9-745D827A8A51}</author>
-    <author>tc={1DF3A368-C5E4-454C-BB52-0ECC3F901258}</author>
   </authors>
   <commentList>
     <comment ref="B388" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -54,22 +52,6 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     10/15/19: Targets not recorded because recording while feeding</t>
-      </text>
-    </comment>
-    <comment ref="A404" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Gray Reefs only ate Salmon. Did not touch Saury.</t>
-      </text>
-    </comment>
-    <comment ref="A408" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Gray Reefs only ate Salmon. Did not touch Saury.</t>
       </text>
     </comment>
   </commentList>
@@ -889,12 +871,6 @@
   <threadedComment ref="B388" dT="2020-09-14T18:28:39.77" personId="{8134DF3D-3BEA-47FD-9D2B-4C443A684911}" id="{88BA8BB9-D010-4657-ACA8-10E27501E5A7}">
     <text>10/15/19: Targets not recorded because recording while feeding</text>
   </threadedComment>
-  <threadedComment ref="A404" dT="2020-09-14T18:57:39.46" personId="{8134DF3D-3BEA-47FD-9D2B-4C443A684911}" id="{E312AADC-0ECB-428F-9DB9-745D827A8A51}">
-    <text>Gray Reefs only ate Salmon. Did not touch Saury.</text>
-  </threadedComment>
-  <threadedComment ref="A408" dT="2020-09-14T19:08:31.90" personId="{8134DF3D-3BEA-47FD-9D2B-4C443A684911}" id="{1DF3A368-C5E4-454C-BB52-0ECC3F901258}">
-    <text>Gray Reefs only ate Salmon. Did not touch Saury.</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -920,8 +896,8 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A309" sqref="A309:A431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25151,8 +25127,8 @@
   <dimension ref="A1:O593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N584" sqref="N584"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A309" sqref="A309:A431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -27077,7 +27053,7 @@
     </row>
     <row r="54" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>39512</v>
+        <v>43164</v>
       </c>
       <c r="B54">
         <v>8</v>
@@ -27410,7 +27386,7 @@
     </row>
     <row r="63" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>42816</v>
+        <v>43181</v>
       </c>
       <c r="B63">
         <v>11</v>
@@ -36251,7 +36227,7 @@
     </row>
     <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" s="5">
-        <v>43981</v>
+        <v>43615</v>
       </c>
       <c r="B309">
         <v>3</v>
@@ -36296,7 +36272,7 @@
     </row>
     <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
-        <v>43983</v>
+        <v>43617</v>
       </c>
       <c r="I310">
         <v>4</v>
@@ -36320,7 +36296,7 @@
     </row>
     <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311" s="5">
-        <v>43984</v>
+        <v>43618</v>
       </c>
       <c r="B311">
         <v>13</v>
@@ -36350,7 +36326,7 @@
     </row>
     <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312" s="5">
-        <v>43986</v>
+        <v>43620</v>
       </c>
       <c r="B312">
         <v>6</v>
@@ -36395,7 +36371,7 @@
     </row>
     <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313" s="5">
-        <v>43988</v>
+        <v>43622</v>
       </c>
       <c r="B313">
         <v>14</v>
@@ -36440,7 +36416,7 @@
     </row>
     <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
-        <v>43990</v>
+        <v>43624</v>
       </c>
       <c r="I314">
         <v>3</v>
@@ -36464,7 +36440,7 @@
     </row>
     <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315" s="5">
-        <v>43991</v>
+        <v>43625</v>
       </c>
       <c r="B315">
         <v>23</v>
@@ -36494,7 +36470,7 @@
     </row>
     <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316" s="5">
-        <v>43993</v>
+        <v>43627</v>
       </c>
       <c r="B316">
         <v>6</v>
@@ -36539,7 +36515,7 @@
     </row>
     <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317" s="5">
-        <v>43995</v>
+        <v>43629</v>
       </c>
       <c r="B317">
         <v>14</v>
@@ -36584,7 +36560,7 @@
     </row>
     <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
-        <v>43997</v>
+        <v>43631</v>
       </c>
       <c r="I318">
         <v>2</v>
@@ -36608,7 +36584,7 @@
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319" s="5">
-        <v>43998</v>
+        <v>43632</v>
       </c>
       <c r="B319">
         <v>25</v>
@@ -36638,7 +36614,7 @@
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320" s="5">
-        <v>44000</v>
+        <v>43634</v>
       </c>
       <c r="B320">
         <v>7</v>
@@ -36683,7 +36659,7 @@
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321" s="5">
-        <v>44002</v>
+        <v>43636</v>
       </c>
       <c r="B321">
         <v>10</v>
@@ -36728,7 +36704,7 @@
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322" s="5">
-        <v>44004</v>
+        <v>43638</v>
       </c>
       <c r="I322">
         <v>5</v>
@@ -36752,7 +36728,7 @@
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323" s="5">
-        <v>44005</v>
+        <v>43639</v>
       </c>
       <c r="B323">
         <v>28</v>
@@ -36782,7 +36758,7 @@
     </row>
     <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
-        <v>44007</v>
+        <v>43641</v>
       </c>
       <c r="B324">
         <v>15</v>
@@ -36827,7 +36803,7 @@
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325" s="5">
-        <v>44009</v>
+        <v>43643</v>
       </c>
       <c r="B325">
         <v>6</v>
@@ -36872,7 +36848,7 @@
     </row>
     <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326" s="5">
-        <v>44011</v>
+        <v>43645</v>
       </c>
       <c r="I326">
         <v>1</v>
@@ -36896,7 +36872,7 @@
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327" s="5">
-        <v>44012</v>
+        <v>43646</v>
       </c>
       <c r="B327">
         <v>14</v>
@@ -36926,7 +36902,7 @@
     </row>
     <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
-        <v>44014</v>
+        <v>43648</v>
       </c>
       <c r="B328">
         <v>14</v>
@@ -36971,7 +36947,7 @@
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
-        <v>44016</v>
+        <v>43650</v>
       </c>
       <c r="B329">
         <v>26</v>
@@ -37016,7 +36992,7 @@
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" s="5">
-        <v>44018</v>
+        <v>43652</v>
       </c>
       <c r="I330">
         <v>4</v>
@@ -37040,7 +37016,7 @@
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
-        <v>43989</v>
+        <v>43653</v>
       </c>
       <c r="B331">
         <v>11</v>
@@ -37070,7 +37046,7 @@
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
-        <v>43991</v>
+        <v>43655</v>
       </c>
       <c r="B332">
         <v>10</v>
@@ -37115,7 +37091,7 @@
     </row>
     <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333" s="5">
-        <v>44023</v>
+        <v>43657</v>
       </c>
       <c r="B333">
         <v>9</v>
@@ -37160,7 +37136,7 @@
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334" s="5">
-        <v>44025</v>
+        <v>43659</v>
       </c>
       <c r="I334">
         <v>1</v>
@@ -37184,7 +37160,7 @@
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335" s="5">
-        <v>44026</v>
+        <v>43660</v>
       </c>
       <c r="B335">
         <v>24</v>
@@ -37214,7 +37190,7 @@
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336" s="5">
-        <v>44028</v>
+        <v>43662</v>
       </c>
       <c r="B336">
         <v>6</v>
@@ -37259,7 +37235,7 @@
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
-        <v>44030</v>
+        <v>43664</v>
       </c>
       <c r="B337">
         <v>9</v>
@@ -37304,7 +37280,7 @@
     </row>
     <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
-        <v>44032</v>
+        <v>43666</v>
       </c>
       <c r="I338">
         <v>1</v>
@@ -37328,7 +37304,7 @@
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
-        <v>44033</v>
+        <v>43667</v>
       </c>
       <c r="B339">
         <v>35</v>
@@ -37358,7 +37334,7 @@
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
-        <v>44035</v>
+        <v>43669</v>
       </c>
       <c r="B340">
         <v>3</v>
@@ -37403,7 +37379,7 @@
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
-        <v>44037</v>
+        <v>43671</v>
       </c>
       <c r="B341">
         <v>32</v>
@@ -37448,7 +37424,7 @@
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
-        <v>44039</v>
+        <v>43673</v>
       </c>
       <c r="I342">
         <v>6</v>
@@ -37472,7 +37448,7 @@
     </row>
     <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
-        <v>44040</v>
+        <v>43674</v>
       </c>
       <c r="B343">
         <v>32</v>
@@ -37502,7 +37478,7 @@
     </row>
     <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
-        <v>44042</v>
+        <v>43676</v>
       </c>
       <c r="B344">
         <v>14</v>
@@ -37547,7 +37523,7 @@
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" s="5">
-        <v>44044</v>
+        <v>43678</v>
       </c>
       <c r="B345">
         <v>3</v>
@@ -37592,7 +37568,7 @@
     </row>
     <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" s="5">
-        <v>44046</v>
+        <v>43680</v>
       </c>
       <c r="I346">
         <v>2</v>
@@ -37616,7 +37592,7 @@
     </row>
     <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" s="5">
-        <v>44047</v>
+        <v>43681</v>
       </c>
       <c r="B347">
         <v>14</v>
@@ -37646,7 +37622,7 @@
     </row>
     <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" s="5">
-        <v>44049</v>
+        <v>43683</v>
       </c>
       <c r="B348">
         <v>4</v>
@@ -37691,7 +37667,7 @@
     </row>
     <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" s="5">
-        <v>44051</v>
+        <v>43685</v>
       </c>
       <c r="B349">
         <v>24</v>
@@ -37736,7 +37712,7 @@
     </row>
     <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350" s="5">
-        <v>44053</v>
+        <v>43687</v>
       </c>
       <c r="I350">
         <v>1</v>
@@ -37760,7 +37736,7 @@
     </row>
     <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351" s="5">
-        <v>44054</v>
+        <v>43688</v>
       </c>
       <c r="B351">
         <v>20</v>
@@ -37790,7 +37766,7 @@
     </row>
     <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352" s="5">
-        <v>44056</v>
+        <v>43690</v>
       </c>
       <c r="B352">
         <v>5</v>
@@ -37835,7 +37811,7 @@
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A353" s="5">
-        <v>44058</v>
+        <v>43692</v>
       </c>
       <c r="B353">
         <v>9</v>
@@ -37880,7 +37856,7 @@
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A354" s="5">
-        <v>44060</v>
+        <v>43694</v>
       </c>
       <c r="I354">
         <v>4</v>
@@ -37904,7 +37880,7 @@
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A355" s="5">
-        <v>44061</v>
+        <v>43695</v>
       </c>
       <c r="B355">
         <v>5</v>
@@ -37934,7 +37910,7 @@
     </row>
     <row r="356" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A356" s="5">
-        <v>44063</v>
+        <v>43697</v>
       </c>
       <c r="B356">
         <v>2</v>
@@ -37979,7 +37955,7 @@
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A357" s="5">
-        <v>44065</v>
+        <v>43699</v>
       </c>
       <c r="B357">
         <v>9</v>
@@ -38024,7 +38000,7 @@
     </row>
     <row r="358" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A358" s="5">
-        <v>44067</v>
+        <v>43701</v>
       </c>
       <c r="I358">
         <v>2</v>
@@ -38048,7 +38024,7 @@
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A359" s="5">
-        <v>44068</v>
+        <v>43702</v>
       </c>
       <c r="B359">
         <v>11</v>
@@ -38078,7 +38054,7 @@
     </row>
     <row r="360" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A360" s="5">
-        <v>44070</v>
+        <v>43704</v>
       </c>
       <c r="B360">
         <v>8</v>
@@ -38123,7 +38099,7 @@
     </row>
     <row r="361" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A361" s="5">
-        <v>44072</v>
+        <v>43706</v>
       </c>
       <c r="B361">
         <v>6</v>
@@ -38168,7 +38144,7 @@
     </row>
     <row r="362" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A362" s="5">
-        <v>44074</v>
+        <v>43708</v>
       </c>
       <c r="I362">
         <v>1</v>
@@ -38192,7 +38168,7 @@
     </row>
     <row r="363" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A363" s="5">
-        <v>44075</v>
+        <v>43709</v>
       </c>
       <c r="B363">
         <v>22</v>
@@ -38222,7 +38198,7 @@
     </row>
     <row r="364" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A364" s="5">
-        <v>44077</v>
+        <v>43711</v>
       </c>
       <c r="B364">
         <v>8</v>
@@ -38267,7 +38243,7 @@
     </row>
     <row r="365" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A365" s="5">
-        <v>44079</v>
+        <v>43713</v>
       </c>
       <c r="B365">
         <v>14</v>
@@ -38312,7 +38288,7 @@
     </row>
     <row r="366" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A366" s="5">
-        <v>44081</v>
+        <v>43715</v>
       </c>
       <c r="I366">
         <v>4</v>
@@ -38336,7 +38312,7 @@
     </row>
     <row r="367" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A367" s="5">
-        <v>44082</v>
+        <v>43716</v>
       </c>
       <c r="B367">
         <v>12</v>
@@ -38366,7 +38342,7 @@
     </row>
     <row r="368" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A368" s="5">
-        <v>44084</v>
+        <v>43718</v>
       </c>
       <c r="B368">
         <v>6</v>
@@ -38411,7 +38387,7 @@
     </row>
     <row r="369" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A369" s="5">
-        <v>44086</v>
+        <v>43720</v>
       </c>
       <c r="B369">
         <v>10</v>
@@ -38456,7 +38432,7 @@
     </row>
     <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370" s="5">
-        <v>44088</v>
+        <v>43722</v>
       </c>
       <c r="I370">
         <v>1</v>
@@ -38480,7 +38456,7 @@
     </row>
     <row r="371" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A371" s="5">
-        <v>44089</v>
+        <v>43723</v>
       </c>
       <c r="B371">
         <v>12</v>
@@ -38510,7 +38486,7 @@
     </row>
     <row r="372" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A372" s="5">
-        <v>44091</v>
+        <v>43725</v>
       </c>
       <c r="B372">
         <v>5</v>
@@ -38555,7 +38531,7 @@
     </row>
     <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373" s="5">
-        <v>44092</v>
+        <v>43726</v>
       </c>
       <c r="B373">
         <v>13</v>
@@ -38600,7 +38576,7 @@
     </row>
     <row r="374" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A374" s="5">
-        <v>44095</v>
+        <v>43729</v>
       </c>
       <c r="I374">
         <v>7</v>
@@ -38624,7 +38600,7 @@
     </row>
     <row r="375" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A375" s="5">
-        <v>44096</v>
+        <v>43730</v>
       </c>
       <c r="B375">
         <v>11</v>
@@ -38654,7 +38630,7 @@
     </row>
     <row r="376" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A376" s="5">
-        <v>44098</v>
+        <v>43732</v>
       </c>
       <c r="B376">
         <v>12</v>
@@ -38699,7 +38675,7 @@
     </row>
     <row r="377" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A377" s="5">
-        <v>44100</v>
+        <v>43734</v>
       </c>
       <c r="B377">
         <v>11</v>
@@ -38744,7 +38720,7 @@
     </row>
     <row r="378" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A378" s="5">
-        <v>44102</v>
+        <v>43736</v>
       </c>
       <c r="I378">
         <v>3</v>
@@ -38768,7 +38744,7 @@
     </row>
     <row r="379" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A379" s="5">
-        <v>44103</v>
+        <v>43737</v>
       </c>
       <c r="B379">
         <v>18</v>
@@ -38798,7 +38774,7 @@
     </row>
     <row r="380" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A380" s="5">
-        <v>44105</v>
+        <v>43739</v>
       </c>
       <c r="B380">
         <v>8</v>
@@ -38843,7 +38819,7 @@
     </row>
     <row r="381" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A381" s="5">
-        <v>44107</v>
+        <v>43741</v>
       </c>
       <c r="B381">
         <v>6</v>
@@ -38888,7 +38864,7 @@
     </row>
     <row r="382" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A382" s="5">
-        <v>44109</v>
+        <v>43743</v>
       </c>
       <c r="I382">
         <v>2</v>
@@ -38912,7 +38888,7 @@
     </row>
     <row r="383" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
-        <v>44110</v>
+        <v>43744</v>
       </c>
       <c r="B383">
         <v>19</v>
@@ -38942,7 +38918,7 @@
     </row>
     <row r="384" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A384" s="5">
-        <v>44112</v>
+        <v>43746</v>
       </c>
       <c r="B384">
         <v>7</v>
@@ -38987,7 +38963,7 @@
     </row>
     <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385" s="5">
-        <v>44114</v>
+        <v>43748</v>
       </c>
       <c r="B385">
         <v>19</v>
@@ -39032,7 +39008,7 @@
     </row>
     <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386" s="5">
-        <v>44116</v>
+        <v>43750</v>
       </c>
       <c r="I386">
         <v>4</v>
@@ -39056,7 +39032,7 @@
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387" s="5">
-        <v>44117</v>
+        <v>43751</v>
       </c>
       <c r="B387">
         <v>16</v>
@@ -39086,7 +39062,7 @@
     </row>
     <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388" s="5">
-        <v>44119</v>
+        <v>43753</v>
       </c>
       <c r="I388">
         <v>3</v>
@@ -39110,7 +39086,7 @@
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389" s="5">
-        <v>44121</v>
+        <v>43755</v>
       </c>
       <c r="B389">
         <v>28</v>
@@ -39155,7 +39131,7 @@
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390" s="5">
-        <v>44123</v>
+        <v>43757</v>
       </c>
       <c r="I390">
         <v>0</v>
@@ -39179,7 +39155,7 @@
     </row>
     <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391" s="5">
-        <v>44124</v>
+        <v>43758</v>
       </c>
       <c r="B391">
         <v>11</v>
@@ -39209,7 +39185,7 @@
     </row>
     <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392" s="5">
-        <v>44126</v>
+        <v>43760</v>
       </c>
       <c r="B392">
         <v>16</v>
@@ -39254,7 +39230,7 @@
     </row>
     <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393" s="5">
-        <v>44128</v>
+        <v>43762</v>
       </c>
       <c r="B393">
         <v>18</v>
@@ -39299,7 +39275,7 @@
     </row>
     <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394" s="5">
-        <v>44130</v>
+        <v>43764</v>
       </c>
       <c r="I394">
         <v>7</v>
@@ -39323,7 +39299,7 @@
     </row>
     <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395" s="5">
-        <v>44132</v>
+        <v>43766</v>
       </c>
       <c r="B395">
         <v>11</v>
@@ -39353,7 +39329,7 @@
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396" s="5">
-        <v>44133</v>
+        <v>43767</v>
       </c>
       <c r="B396">
         <v>4</v>
@@ -39398,7 +39374,7 @@
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A397" s="5">
-        <v>44135</v>
+        <v>43769</v>
       </c>
       <c r="B397">
         <v>11</v>
@@ -39443,7 +39419,7 @@
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A398" s="5">
-        <v>44137</v>
+        <v>43771</v>
       </c>
       <c r="I398">
         <v>4</v>
@@ -39467,7 +39443,7 @@
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A399" s="5">
-        <v>44138</v>
+        <v>43772</v>
       </c>
       <c r="B399">
         <v>3</v>
@@ -39497,7 +39473,7 @@
     </row>
     <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A400" s="5">
-        <v>44140</v>
+        <v>43774</v>
       </c>
       <c r="B400">
         <v>3</v>
@@ -39542,7 +39518,7 @@
     </row>
     <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401" s="5">
-        <v>44142</v>
+        <v>43776</v>
       </c>
       <c r="B401">
         <v>3</v>
@@ -39587,7 +39563,7 @@
     </row>
     <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402" s="5">
-        <v>44144</v>
+        <v>43778</v>
       </c>
       <c r="I402">
         <v>6</v>
@@ -39611,7 +39587,7 @@
     </row>
     <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403" s="5">
-        <v>44145</v>
+        <v>43779</v>
       </c>
       <c r="B403">
         <v>19</v>
@@ -39641,7 +39617,7 @@
     </row>
     <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
-        <v>44147</v>
+        <v>43781</v>
       </c>
       <c r="B404">
         <v>14</v>
@@ -39686,7 +39662,7 @@
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405" s="5">
-        <v>44149</v>
+        <v>43783</v>
       </c>
       <c r="B405">
         <v>5</v>
@@ -39731,7 +39707,7 @@
     </row>
     <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406" s="5">
-        <v>44151</v>
+        <v>43785</v>
       </c>
       <c r="I406">
         <v>1</v>
@@ -39755,7 +39731,7 @@
     </row>
     <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407" s="5">
-        <v>44152</v>
+        <v>43786</v>
       </c>
       <c r="B407">
         <v>27</v>
@@ -39785,7 +39761,7 @@
     </row>
     <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408" s="5">
-        <v>44154</v>
+        <v>43788</v>
       </c>
       <c r="B408">
         <v>6</v>
@@ -39830,7 +39806,7 @@
     </row>
     <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409" s="5">
-        <v>44156</v>
+        <v>43790</v>
       </c>
       <c r="B409">
         <v>6</v>
@@ -39875,7 +39851,7 @@
     </row>
     <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410" s="5">
-        <v>44158</v>
+        <v>43792</v>
       </c>
       <c r="I410">
         <v>4</v>
@@ -39899,7 +39875,7 @@
     </row>
     <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411" s="5">
-        <v>44159</v>
+        <v>43793</v>
       </c>
       <c r="B411">
         <v>9</v>
@@ -39929,7 +39905,7 @@
     </row>
     <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412" s="5">
-        <v>44161</v>
+        <v>43795</v>
       </c>
       <c r="B412">
         <v>14</v>
@@ -39974,7 +39950,7 @@
     </row>
     <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413" s="5">
-        <v>44165</v>
+        <v>43799</v>
       </c>
       <c r="I413">
         <v>5</v>
@@ -39998,7 +39974,7 @@
     </row>
     <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414" s="5">
-        <v>44166</v>
+        <v>43800</v>
       </c>
       <c r="B414">
         <v>8</v>
@@ -40028,7 +40004,7 @@
     </row>
     <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415" s="5">
-        <v>44168</v>
+        <v>43802</v>
       </c>
       <c r="B415">
         <v>9</v>
@@ -40073,7 +40049,7 @@
     </row>
     <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416" s="5">
-        <v>44170</v>
+        <v>43804</v>
       </c>
       <c r="B416">
         <v>5</v>
@@ -40118,7 +40094,7 @@
     </row>
     <row r="417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A417" s="5">
-        <v>44172</v>
+        <v>43806</v>
       </c>
       <c r="I417">
         <v>3</v>
@@ -40142,7 +40118,7 @@
     </row>
     <row r="418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A418" s="5">
-        <v>44173</v>
+        <v>43807</v>
       </c>
       <c r="B418">
         <v>7</v>
@@ -40172,7 +40148,7 @@
     </row>
     <row r="419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A419" s="5">
-        <v>44175</v>
+        <v>43809</v>
       </c>
       <c r="B419">
         <v>8</v>
@@ -40217,7 +40193,7 @@
     </row>
     <row r="420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A420" s="5">
-        <v>44177</v>
+        <v>43811</v>
       </c>
       <c r="B420">
         <v>2</v>
@@ -40262,7 +40238,7 @@
     </row>
     <row r="421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
-        <v>44180</v>
+        <v>43814</v>
       </c>
       <c r="I421">
         <v>4</v>
@@ -40286,7 +40262,7 @@
     </row>
     <row r="422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A422" s="5">
-        <v>44181</v>
+        <v>43815</v>
       </c>
       <c r="B422">
         <v>8</v>
@@ -40316,7 +40292,7 @@
     </row>
     <row r="423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A423" s="5">
-        <v>44182</v>
+        <v>43816</v>
       </c>
       <c r="B423">
         <v>8</v>
@@ -40361,7 +40337,7 @@
     </row>
     <row r="424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A424" s="5">
-        <v>44184</v>
+        <v>43818</v>
       </c>
       <c r="B424">
         <v>8</v>
@@ -40406,7 +40382,7 @@
     </row>
     <row r="425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A425" s="5">
-        <v>44186</v>
+        <v>43820</v>
       </c>
       <c r="I425">
         <v>7</v>
@@ -40430,7 +40406,7 @@
     </row>
     <row r="426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A426" s="5">
-        <v>44187</v>
+        <v>43821</v>
       </c>
       <c r="B426">
         <v>9</v>
@@ -40460,7 +40436,7 @@
     </row>
     <row r="427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A427" s="5">
-        <v>44189</v>
+        <v>43823</v>
       </c>
       <c r="B427">
         <v>1</v>
@@ -40505,7 +40481,7 @@
     </row>
     <row r="428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A428" s="5">
-        <v>44191</v>
+        <v>43825</v>
       </c>
       <c r="B428">
         <v>13</v>
@@ -40550,7 +40526,7 @@
     </row>
     <row r="429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A429" s="5">
-        <v>44193</v>
+        <v>43827</v>
       </c>
       <c r="I429">
         <v>1</v>
@@ -40574,7 +40550,7 @@
     </row>
     <row r="430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A430" s="5">
-        <v>44194</v>
+        <v>43828</v>
       </c>
       <c r="B430">
         <v>8</v>
@@ -40604,7 +40580,7 @@
     </row>
     <row r="431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A431" s="5">
-        <v>44196</v>
+        <v>43830</v>
       </c>
       <c r="B431">
         <v>6</v>
@@ -46244,8 +46220,8 @@
   <dimension ref="A1:O593"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E322" sqref="E322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -57359,7 +57335,7 @@
     </row>
     <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" s="5">
-        <v>43981</v>
+        <v>43615</v>
       </c>
       <c r="B309">
         <v>0</v>
@@ -57404,7 +57380,7 @@
     </row>
     <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
-        <v>43983</v>
+        <v>43617</v>
       </c>
       <c r="I310">
         <v>0</v>
@@ -57428,7 +57404,7 @@
     </row>
     <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311" s="5">
-        <v>43984</v>
+        <v>43618</v>
       </c>
       <c r="B311">
         <v>0</v>
@@ -57458,7 +57434,7 @@
     </row>
     <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312" s="5">
-        <v>43986</v>
+        <v>43620</v>
       </c>
       <c r="B312">
         <v>0</v>
@@ -57503,7 +57479,7 @@
     </row>
     <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313" s="5">
-        <v>43988</v>
+        <v>43622</v>
       </c>
       <c r="B313">
         <v>1</v>
@@ -57548,7 +57524,7 @@
     </row>
     <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
-        <v>43990</v>
+        <v>43624</v>
       </c>
       <c r="I314">
         <v>0</v>
@@ -57572,7 +57548,7 @@
     </row>
     <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315" s="5">
-        <v>43991</v>
+        <v>43625</v>
       </c>
       <c r="B315">
         <v>0</v>
@@ -57602,7 +57578,7 @@
     </row>
     <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316" s="5">
-        <v>43993</v>
+        <v>43627</v>
       </c>
       <c r="B316">
         <v>1</v>
@@ -57647,7 +57623,7 @@
     </row>
     <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317" s="5">
-        <v>43995</v>
+        <v>43629</v>
       </c>
       <c r="B317">
         <v>0</v>
@@ -57692,7 +57668,7 @@
     </row>
     <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
-        <v>43997</v>
+        <v>43631</v>
       </c>
       <c r="I318">
         <v>0</v>
@@ -57716,7 +57692,7 @@
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319" s="5">
-        <v>43998</v>
+        <v>43632</v>
       </c>
       <c r="B319">
         <v>0</v>
@@ -57746,7 +57722,7 @@
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320" s="5">
-        <v>44000</v>
+        <v>43634</v>
       </c>
       <c r="B320">
         <v>1</v>
@@ -57791,7 +57767,7 @@
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321" s="5">
-        <v>44002</v>
+        <v>43636</v>
       </c>
       <c r="B321">
         <v>0</v>
@@ -57836,7 +57812,7 @@
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322" s="5">
-        <v>44004</v>
+        <v>43638</v>
       </c>
       <c r="I322">
         <v>0</v>
@@ -57860,7 +57836,7 @@
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323" s="5">
-        <v>44005</v>
+        <v>43639</v>
       </c>
       <c r="B323">
         <v>1</v>
@@ -57890,7 +57866,7 @@
     </row>
     <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
-        <v>44007</v>
+        <v>43641</v>
       </c>
       <c r="B324">
         <v>0</v>
@@ -57935,7 +57911,7 @@
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325" s="5">
-        <v>44009</v>
+        <v>43643</v>
       </c>
       <c r="B325">
         <v>0</v>
@@ -57980,7 +57956,7 @@
     </row>
     <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326" s="5">
-        <v>44011</v>
+        <v>43645</v>
       </c>
       <c r="I326">
         <v>0</v>
@@ -58004,7 +57980,7 @@
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327" s="5">
-        <v>44012</v>
+        <v>43646</v>
       </c>
       <c r="B327">
         <v>0</v>
@@ -58034,7 +58010,7 @@
     </row>
     <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
-        <v>44014</v>
+        <v>43648</v>
       </c>
       <c r="B328">
         <v>0</v>
@@ -58079,7 +58055,7 @@
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
-        <v>44016</v>
+        <v>43650</v>
       </c>
       <c r="B329">
         <v>0</v>
@@ -58124,7 +58100,7 @@
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" s="5">
-        <v>44018</v>
+        <v>43652</v>
       </c>
       <c r="I330">
         <v>0</v>
@@ -58148,7 +58124,7 @@
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
-        <v>43989</v>
+        <v>43653</v>
       </c>
       <c r="B331">
         <v>0</v>
@@ -58178,7 +58154,7 @@
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
-        <v>43991</v>
+        <v>43655</v>
       </c>
       <c r="B332">
         <v>0</v>
@@ -58223,7 +58199,7 @@
     </row>
     <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333" s="5">
-        <v>44023</v>
+        <v>43657</v>
       </c>
       <c r="B333">
         <v>1</v>
@@ -58268,7 +58244,7 @@
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334" s="5">
-        <v>44025</v>
+        <v>43659</v>
       </c>
       <c r="I334">
         <v>0</v>
@@ -58292,7 +58268,7 @@
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335" s="5">
-        <v>44026</v>
+        <v>43660</v>
       </c>
       <c r="B335">
         <v>0</v>
@@ -58322,7 +58298,7 @@
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336" s="5">
-        <v>44028</v>
+        <v>43662</v>
       </c>
       <c r="B336">
         <v>0</v>
@@ -58367,7 +58343,7 @@
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
-        <v>44030</v>
+        <v>43664</v>
       </c>
       <c r="B337">
         <v>0</v>
@@ -58412,7 +58388,7 @@
     </row>
     <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
-        <v>44032</v>
+        <v>43666</v>
       </c>
       <c r="I338">
         <v>1</v>
@@ -58436,7 +58412,7 @@
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
-        <v>44033</v>
+        <v>43667</v>
       </c>
       <c r="B339">
         <v>0</v>
@@ -58466,7 +58442,7 @@
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
-        <v>44035</v>
+        <v>43669</v>
       </c>
       <c r="B340">
         <v>0</v>
@@ -58511,7 +58487,7 @@
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
-        <v>44037</v>
+        <v>43671</v>
       </c>
       <c r="B341">
         <v>0</v>
@@ -58556,7 +58532,7 @@
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
-        <v>44039</v>
+        <v>43673</v>
       </c>
       <c r="I342">
         <v>0</v>
@@ -58580,7 +58556,7 @@
     </row>
     <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
-        <v>44040</v>
+        <v>43674</v>
       </c>
       <c r="B343">
         <v>0</v>
@@ -58610,7 +58586,7 @@
     </row>
     <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
-        <v>44042</v>
+        <v>43676</v>
       </c>
       <c r="B344">
         <v>0</v>
@@ -58655,7 +58631,7 @@
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" s="5">
-        <v>44044</v>
+        <v>43678</v>
       </c>
       <c r="B345">
         <v>1</v>
@@ -58700,7 +58676,7 @@
     </row>
     <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" s="5">
-        <v>44046</v>
+        <v>43680</v>
       </c>
       <c r="I346">
         <v>0</v>
@@ -58724,7 +58700,7 @@
     </row>
     <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" s="5">
-        <v>44047</v>
+        <v>43681</v>
       </c>
       <c r="B347">
         <v>1</v>
@@ -58754,7 +58730,7 @@
     </row>
     <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" s="5">
-        <v>44049</v>
+        <v>43683</v>
       </c>
       <c r="B348">
         <v>0</v>
@@ -58799,7 +58775,7 @@
     </row>
     <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" s="5">
-        <v>44051</v>
+        <v>43685</v>
       </c>
       <c r="B349">
         <v>0</v>
@@ -58844,7 +58820,7 @@
     </row>
     <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350" s="5">
-        <v>44053</v>
+        <v>43687</v>
       </c>
       <c r="I350">
         <v>0</v>
@@ -58868,7 +58844,7 @@
     </row>
     <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351" s="5">
-        <v>44054</v>
+        <v>43688</v>
       </c>
       <c r="B351">
         <v>0</v>
@@ -58898,7 +58874,7 @@
     </row>
     <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352" s="5">
-        <v>44056</v>
+        <v>43690</v>
       </c>
       <c r="B352">
         <v>0</v>
@@ -58943,7 +58919,7 @@
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A353" s="5">
-        <v>44058</v>
+        <v>43692</v>
       </c>
       <c r="B353">
         <v>0</v>
@@ -58988,7 +58964,7 @@
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A354" s="5">
-        <v>44060</v>
+        <v>43694</v>
       </c>
       <c r="I354">
         <v>0</v>
@@ -59012,7 +58988,7 @@
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A355" s="5">
-        <v>44061</v>
+        <v>43695</v>
       </c>
       <c r="B355">
         <v>0</v>
@@ -59042,7 +59018,7 @@
     </row>
     <row r="356" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A356" s="5">
-        <v>44063</v>
+        <v>43697</v>
       </c>
       <c r="B356">
         <v>0</v>
@@ -59087,7 +59063,7 @@
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A357" s="5">
-        <v>44065</v>
+        <v>43699</v>
       </c>
       <c r="B357">
         <v>0</v>
@@ -59132,7 +59108,7 @@
     </row>
     <row r="358" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A358" s="5">
-        <v>44067</v>
+        <v>43701</v>
       </c>
       <c r="I358">
         <v>1</v>
@@ -59156,7 +59132,7 @@
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A359" s="5">
-        <v>44068</v>
+        <v>43702</v>
       </c>
       <c r="B359">
         <v>0</v>
@@ -59186,7 +59162,7 @@
     </row>
     <row r="360" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A360" s="5">
-        <v>44070</v>
+        <v>43704</v>
       </c>
       <c r="B360">
         <v>0</v>
@@ -59231,7 +59207,7 @@
     </row>
     <row r="361" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A361" s="5">
-        <v>44072</v>
+        <v>43706</v>
       </c>
       <c r="B361">
         <v>0</v>
@@ -59276,7 +59252,7 @@
     </row>
     <row r="362" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A362" s="5">
-        <v>44074</v>
+        <v>43708</v>
       </c>
       <c r="I362">
         <v>0</v>
@@ -59300,7 +59276,7 @@
     </row>
     <row r="363" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A363" s="5">
-        <v>44075</v>
+        <v>43709</v>
       </c>
       <c r="B363">
         <v>1</v>
@@ -59330,7 +59306,7 @@
     </row>
     <row r="364" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A364" s="5">
-        <v>44077</v>
+        <v>43711</v>
       </c>
       <c r="B364">
         <v>0</v>
@@ -59375,7 +59351,7 @@
     </row>
     <row r="365" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A365" s="5">
-        <v>44079</v>
+        <v>43713</v>
       </c>
       <c r="B365">
         <v>0</v>
@@ -59420,7 +59396,7 @@
     </row>
     <row r="366" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A366" s="5">
-        <v>44081</v>
+        <v>43715</v>
       </c>
       <c r="I366">
         <v>0</v>
@@ -59444,7 +59420,7 @@
     </row>
     <row r="367" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A367" s="5">
-        <v>44082</v>
+        <v>43716</v>
       </c>
       <c r="B367">
         <v>0</v>
@@ -59474,7 +59450,7 @@
     </row>
     <row r="368" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A368" s="5">
-        <v>44084</v>
+        <v>43718</v>
       </c>
       <c r="B368">
         <v>0</v>
@@ -59519,7 +59495,7 @@
     </row>
     <row r="369" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A369" s="5">
-        <v>44086</v>
+        <v>43720</v>
       </c>
       <c r="B369">
         <v>0</v>
@@ -59564,7 +59540,7 @@
     </row>
     <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370" s="5">
-        <v>44088</v>
+        <v>43722</v>
       </c>
       <c r="I370">
         <v>1</v>
@@ -59588,7 +59564,7 @@
     </row>
     <row r="371" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A371" s="5">
-        <v>44089</v>
+        <v>43723</v>
       </c>
       <c r="B371">
         <v>0</v>
@@ -59618,7 +59594,7 @@
     </row>
     <row r="372" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A372" s="5">
-        <v>44091</v>
+        <v>43725</v>
       </c>
       <c r="B372">
         <v>0</v>
@@ -59663,7 +59639,7 @@
     </row>
     <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373" s="5">
-        <v>44092</v>
+        <v>43726</v>
       </c>
       <c r="B373">
         <v>0</v>
@@ -59708,7 +59684,7 @@
     </row>
     <row r="374" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A374" s="5">
-        <v>44095</v>
+        <v>43729</v>
       </c>
       <c r="I374">
         <v>0</v>
@@ -59732,7 +59708,7 @@
     </row>
     <row r="375" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A375" s="5">
-        <v>44096</v>
+        <v>43730</v>
       </c>
       <c r="B375">
         <v>2</v>
@@ -59762,7 +59738,7 @@
     </row>
     <row r="376" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A376" s="5">
-        <v>44098</v>
+        <v>43732</v>
       </c>
       <c r="B376">
         <v>0</v>
@@ -59807,7 +59783,7 @@
     </row>
     <row r="377" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A377" s="5">
-        <v>44100</v>
+        <v>43734</v>
       </c>
       <c r="B377">
         <v>0</v>
@@ -59852,7 +59828,7 @@
     </row>
     <row r="378" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A378" s="5">
-        <v>44102</v>
+        <v>43736</v>
       </c>
       <c r="I378">
         <v>0</v>
@@ -59876,7 +59852,7 @@
     </row>
     <row r="379" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A379" s="5">
-        <v>44103</v>
+        <v>43737</v>
       </c>
       <c r="B379">
         <v>0</v>
@@ -59906,7 +59882,7 @@
     </row>
     <row r="380" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A380" s="5">
-        <v>44105</v>
+        <v>43739</v>
       </c>
       <c r="B380">
         <v>0</v>
@@ -59951,7 +59927,7 @@
     </row>
     <row r="381" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A381" s="5">
-        <v>44107</v>
+        <v>43741</v>
       </c>
       <c r="B381">
         <v>1</v>
@@ -59996,7 +59972,7 @@
     </row>
     <row r="382" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A382" s="5">
-        <v>44109</v>
+        <v>43743</v>
       </c>
       <c r="I382">
         <v>0</v>
@@ -60020,7 +59996,7 @@
     </row>
     <row r="383" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
-        <v>44110</v>
+        <v>43744</v>
       </c>
       <c r="B383">
         <v>0</v>
@@ -60050,7 +60026,7 @@
     </row>
     <row r="384" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A384" s="5">
-        <v>44112</v>
+        <v>43746</v>
       </c>
       <c r="B384">
         <v>0</v>
@@ -60095,7 +60071,7 @@
     </row>
     <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385" s="5">
-        <v>44114</v>
+        <v>43748</v>
       </c>
       <c r="B385">
         <v>0</v>
@@ -60140,7 +60116,7 @@
     </row>
     <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386" s="5">
-        <v>44116</v>
+        <v>43750</v>
       </c>
       <c r="I386">
         <v>0</v>
@@ -60164,7 +60140,7 @@
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387" s="5">
-        <v>44117</v>
+        <v>43751</v>
       </c>
       <c r="B387">
         <v>0</v>
@@ -60194,7 +60170,7 @@
     </row>
     <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388" s="5">
-        <v>44119</v>
+        <v>43753</v>
       </c>
       <c r="B388">
         <v>1</v>
@@ -60239,7 +60215,7 @@
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389" s="5">
-        <v>44121</v>
+        <v>43755</v>
       </c>
       <c r="B389">
         <v>0</v>
@@ -60284,7 +60260,7 @@
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390" s="5">
-        <v>44123</v>
+        <v>43757</v>
       </c>
       <c r="I390">
         <v>1</v>
@@ -60308,7 +60284,7 @@
     </row>
     <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391" s="5">
-        <v>44124</v>
+        <v>43758</v>
       </c>
       <c r="B391">
         <v>0</v>
@@ -60338,7 +60314,7 @@
     </row>
     <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392" s="5">
-        <v>44126</v>
+        <v>43760</v>
       </c>
       <c r="B392">
         <v>0</v>
@@ -60383,7 +60359,7 @@
     </row>
     <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393" s="5">
-        <v>44128</v>
+        <v>43762</v>
       </c>
       <c r="B393">
         <v>0</v>
@@ -60428,7 +60404,7 @@
     </row>
     <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394" s="5">
-        <v>44130</v>
+        <v>43764</v>
       </c>
       <c r="I394">
         <v>0</v>
@@ -60452,7 +60428,7 @@
     </row>
     <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395" s="5">
-        <v>44132</v>
+        <v>43766</v>
       </c>
       <c r="B395">
         <v>0</v>
@@ -60482,7 +60458,7 @@
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396" s="5">
-        <v>44133</v>
+        <v>43767</v>
       </c>
       <c r="B396">
         <v>0</v>
@@ -60527,7 +60503,7 @@
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A397" s="5">
-        <v>44135</v>
+        <v>43769</v>
       </c>
       <c r="B397">
         <v>1</v>
@@ -60572,7 +60548,7 @@
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A398" s="5">
-        <v>44137</v>
+        <v>43771</v>
       </c>
       <c r="I398">
         <v>0</v>
@@ -60596,7 +60572,7 @@
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A399" s="5">
-        <v>44138</v>
+        <v>43772</v>
       </c>
       <c r="B399">
         <v>0</v>
@@ -60626,7 +60602,7 @@
     </row>
     <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A400" s="5">
-        <v>44140</v>
+        <v>43774</v>
       </c>
       <c r="B400">
         <v>0</v>
@@ -60671,7 +60647,7 @@
     </row>
     <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401" s="5">
-        <v>44142</v>
+        <v>43776</v>
       </c>
       <c r="B401">
         <v>0</v>
@@ -60716,7 +60692,7 @@
     </row>
     <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402" s="5">
-        <v>44144</v>
+        <v>43778</v>
       </c>
       <c r="I402">
         <v>0</v>
@@ -60740,7 +60716,7 @@
     </row>
     <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403" s="5">
-        <v>44145</v>
+        <v>43779</v>
       </c>
       <c r="B403">
         <v>0</v>
@@ -60770,7 +60746,7 @@
     </row>
     <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
-        <v>44147</v>
+        <v>43781</v>
       </c>
       <c r="B404">
         <v>0</v>
@@ -60815,7 +60791,7 @@
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405" s="5">
-        <v>44149</v>
+        <v>43783</v>
       </c>
       <c r="B405">
         <v>0</v>
@@ -60860,7 +60836,7 @@
     </row>
     <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406" s="5">
-        <v>44151</v>
+        <v>43785</v>
       </c>
       <c r="I406">
         <v>0</v>
@@ -60884,7 +60860,7 @@
     </row>
     <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407" s="5">
-        <v>44152</v>
+        <v>43786</v>
       </c>
       <c r="B407">
         <v>0</v>
@@ -60914,7 +60890,7 @@
     </row>
     <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408" s="5">
-        <v>44154</v>
+        <v>43788</v>
       </c>
       <c r="B408">
         <v>0</v>
@@ -60959,7 +60935,7 @@
     </row>
     <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409" s="5">
-        <v>44156</v>
+        <v>43790</v>
       </c>
       <c r="B409">
         <v>0</v>
@@ -61004,7 +60980,7 @@
     </row>
     <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410" s="5">
-        <v>44158</v>
+        <v>43792</v>
       </c>
       <c r="I410">
         <v>1</v>
@@ -61028,7 +61004,7 @@
     </row>
     <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411" s="5">
-        <v>44159</v>
+        <v>43793</v>
       </c>
       <c r="B411">
         <v>0</v>
@@ -61058,7 +61034,7 @@
     </row>
     <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412" s="5">
-        <v>44161</v>
+        <v>43795</v>
       </c>
       <c r="B412">
         <v>0</v>
@@ -61103,7 +61079,7 @@
     </row>
     <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413" s="5">
-        <v>44165</v>
+        <v>43799</v>
       </c>
       <c r="I413">
         <v>0</v>
@@ -61127,7 +61103,7 @@
     </row>
     <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414" s="5">
-        <v>44166</v>
+        <v>43800</v>
       </c>
       <c r="B414">
         <v>0</v>
@@ -61157,7 +61133,7 @@
     </row>
     <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415" s="5">
-        <v>44168</v>
+        <v>43802</v>
       </c>
       <c r="B415">
         <v>0</v>
@@ -61202,7 +61178,7 @@
     </row>
     <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416" s="5">
-        <v>44170</v>
+        <v>43804</v>
       </c>
       <c r="B416">
         <v>0</v>
@@ -61247,7 +61223,7 @@
     </row>
     <row r="417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A417" s="5">
-        <v>44172</v>
+        <v>43806</v>
       </c>
       <c r="I417">
         <v>0</v>
@@ -61271,7 +61247,7 @@
     </row>
     <row r="418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A418" s="5">
-        <v>44173</v>
+        <v>43807</v>
       </c>
       <c r="B418">
         <v>0</v>
@@ -61301,7 +61277,7 @@
     </row>
     <row r="419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A419" s="5">
-        <v>44175</v>
+        <v>43809</v>
       </c>
       <c r="B419">
         <v>0</v>
@@ -61346,7 +61322,7 @@
     </row>
     <row r="420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A420" s="5">
-        <v>44177</v>
+        <v>43811</v>
       </c>
       <c r="B420">
         <v>0</v>
@@ -61391,7 +61367,7 @@
     </row>
     <row r="421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
-        <v>44180</v>
+        <v>43814</v>
       </c>
       <c r="I421">
         <v>2</v>
@@ -61415,7 +61391,7 @@
     </row>
     <row r="422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A422" s="5">
-        <v>44181</v>
+        <v>43815</v>
       </c>
       <c r="B422">
         <v>1</v>
@@ -61445,7 +61421,7 @@
     </row>
     <row r="423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A423" s="5">
-        <v>44182</v>
+        <v>43816</v>
       </c>
       <c r="B423">
         <v>0</v>
@@ -61490,7 +61466,7 @@
     </row>
     <row r="424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A424" s="5">
-        <v>44184</v>
+        <v>43818</v>
       </c>
       <c r="B424">
         <v>0</v>
@@ -61535,7 +61511,7 @@
     </row>
     <row r="425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A425" s="5">
-        <v>44186</v>
+        <v>43820</v>
       </c>
       <c r="I425">
         <v>0</v>
@@ -61559,7 +61535,7 @@
     </row>
     <row r="426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A426" s="5">
-        <v>44187</v>
+        <v>43821</v>
       </c>
       <c r="B426">
         <v>0</v>
@@ -61589,7 +61565,7 @@
     </row>
     <row r="427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A427" s="5">
-        <v>44189</v>
+        <v>43823</v>
       </c>
       <c r="B427">
         <v>0</v>
@@ -61634,7 +61610,7 @@
     </row>
     <row r="428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A428" s="5">
-        <v>44191</v>
+        <v>43825</v>
       </c>
       <c r="B428">
         <v>0</v>
@@ -61679,7 +61655,7 @@
     </row>
     <row r="429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A429" s="5">
-        <v>44193</v>
+        <v>43827</v>
       </c>
       <c r="I429">
         <v>1</v>
@@ -61703,7 +61679,7 @@
     </row>
     <row r="430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A430" s="5">
-        <v>44194</v>
+        <v>43828</v>
       </c>
       <c r="B430">
         <v>0</v>
@@ -61733,7 +61709,7 @@
     </row>
     <row r="431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A431" s="5">
-        <v>44196</v>
+        <v>43830</v>
       </c>
       <c r="B431">
         <v>0</v>

</xml_diff>

<commit_message>
Had to change some incorrect dates. I also made some minor changes in Poisson. Mostly I worked on the T-tests for right before corona vs. corona and I added those graphs to the presentation
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/753f33f7ae04b4eb/Documents/Fall 2020/Stat 495R/final-project-danny_brady_michael/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55C1D362-3F6B-40E7-85A7-B2CD78818E77}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69618D21-8C0B-44B8-9C0B-1BAB8B51074F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces Eaten" sheetId="1" r:id="rId1"/>
@@ -584,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -610,10 +610,8 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -895,9 +893,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A309" sqref="A309:A431"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23456,13 +23454,13 @@
       <c r="A578" s="22">
         <v>44093</v>
       </c>
-      <c r="B578" s="32"/>
-      <c r="C578" s="32"/>
-      <c r="D578" s="32"/>
-      <c r="E578" s="32"/>
-      <c r="F578" s="32"/>
-      <c r="G578" s="32"/>
-      <c r="H578" s="32"/>
+      <c r="B578" s="30"/>
+      <c r="C578" s="30"/>
+      <c r="D578" s="30"/>
+      <c r="E578" s="30"/>
+      <c r="F578" s="30"/>
+      <c r="G578" s="30"/>
+      <c r="H578" s="30"/>
       <c r="I578" s="1">
         <v>2</v>
       </c>
@@ -23484,31 +23482,31 @@
       </c>
     </row>
     <row r="579" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A579" s="30">
+      <c r="A579" s="28">
         <v>44094</v>
       </c>
-      <c r="B579" s="29">
-        <v>4</v>
-      </c>
-      <c r="C579" s="29">
+      <c r="B579" s="27">
+        <v>4</v>
+      </c>
+      <c r="C579" s="27">
         <v>6</v>
       </c>
-      <c r="D579" s="29">
-        <v>0</v>
-      </c>
-      <c r="E579" s="29">
-        <v>1</v>
-      </c>
-      <c r="F579" s="29">
-        <v>1</v>
-      </c>
-      <c r="G579" s="29">
-        <v>1</v>
-      </c>
-      <c r="H579" s="29">
-        <v>4</v>
-      </c>
-      <c r="I579" s="31"/>
+      <c r="D579" s="27">
+        <v>0</v>
+      </c>
+      <c r="E579" s="27">
+        <v>1</v>
+      </c>
+      <c r="F579" s="27">
+        <v>1</v>
+      </c>
+      <c r="G579" s="27">
+        <v>1</v>
+      </c>
+      <c r="H579" s="27">
+        <v>4</v>
+      </c>
+      <c r="I579" s="29"/>
       <c r="J579" s="1"/>
       <c r="K579" s="1"/>
       <c r="L579" s="1"/>
@@ -23522,25 +23520,25 @@
       <c r="A580" s="22">
         <v>44096</v>
       </c>
-      <c r="B580" s="33">
+      <c r="B580" s="31">
         <v>6</v>
       </c>
-      <c r="C580" s="33">
-        <v>0</v>
-      </c>
-      <c r="D580" s="33">
-        <v>1</v>
-      </c>
-      <c r="E580" s="33">
-        <v>2</v>
-      </c>
-      <c r="F580" s="33">
+      <c r="C580" s="31">
+        <v>0</v>
+      </c>
+      <c r="D580" s="31">
+        <v>1</v>
+      </c>
+      <c r="E580" s="31">
+        <v>2</v>
+      </c>
+      <c r="F580" s="31">
         <v>6</v>
       </c>
-      <c r="G580" s="33">
-        <v>0</v>
-      </c>
-      <c r="H580" s="33">
+      <c r="G580" s="31">
+        <v>0</v>
+      </c>
+      <c r="H580" s="31">
         <v>4</v>
       </c>
       <c r="I580" s="1">
@@ -25127,8 +25125,8 @@
   <dimension ref="A1:O593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A309" sqref="A309:A431"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -25877,7 +25875,7 @@
     </row>
     <row r="22" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>43472</v>
+        <v>43107</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -27863,7 +27861,7 @@
     </row>
     <row r="76" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>43935</v>
+        <v>43204</v>
       </c>
       <c r="I76">
         <v>3</v>
@@ -31052,7 +31050,7 @@
     </row>
     <row r="165" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
-        <v>43724</v>
+        <v>43359</v>
       </c>
       <c r="B165">
         <v>5</v>
@@ -31916,7 +31914,7 @@
     </row>
     <row r="189" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
-        <v>43766</v>
+        <v>43401</v>
       </c>
       <c r="B189">
         <v>13</v>
@@ -32204,7 +32202,7 @@
     </row>
     <row r="197" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
-        <v>43780</v>
+        <v>43415</v>
       </c>
       <c r="B197">
         <v>6</v>
@@ -35408,7 +35406,7 @@
     </row>
     <row r="286" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A286" s="3">
-        <v>43210</v>
+        <v>43575</v>
       </c>
       <c r="I286">
         <v>0</v>
@@ -45959,28 +45957,28 @@
       </c>
     </row>
     <row r="579" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A579" s="30">
+      <c r="A579" s="28">
         <v>44094</v>
       </c>
-      <c r="B579" s="34">
-        <v>2</v>
-      </c>
-      <c r="C579" s="34">
+      <c r="B579" s="32">
+        <v>2</v>
+      </c>
+      <c r="C579" s="32">
         <v>9</v>
       </c>
-      <c r="D579" s="34">
+      <c r="D579" s="32">
         <v>6</v>
       </c>
-      <c r="E579" s="34">
+      <c r="E579" s="32">
         <v>7</v>
       </c>
-      <c r="F579" s="34">
-        <v>5</v>
-      </c>
-      <c r="G579" s="34">
-        <v>3</v>
-      </c>
-      <c r="H579" s="34">
+      <c r="F579" s="32">
+        <v>5</v>
+      </c>
+      <c r="G579" s="32">
+        <v>3</v>
+      </c>
+      <c r="H579" s="32">
         <v>6</v>
       </c>
       <c r="N579">
@@ -46219,9 +46217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O593"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E322" sqref="E322"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -46970,7 +46968,7 @@
     </row>
     <row r="22" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>43472</v>
+        <v>43107</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -48956,7 +48954,7 @@
     </row>
     <row r="76" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>43935</v>
+        <v>43204</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -52160,7 +52158,7 @@
     </row>
     <row r="165" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
-        <v>43724</v>
+        <v>43359</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -53024,7 +53022,7 @@
     </row>
     <row r="189" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
-        <v>43766</v>
+        <v>43401</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -53312,7 +53310,7 @@
     </row>
     <row r="197" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
-        <v>43780</v>
+        <v>43415</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -56516,7 +56514,7 @@
     </row>
     <row r="286" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A286" s="3">
-        <v>43210</v>
+        <v>43575</v>
       </c>
       <c r="I286">
         <v>0</v>
@@ -67082,7 +67080,7 @@
       </c>
     </row>
     <row r="579" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A579" s="30">
+      <c r="A579" s="28">
         <v>44094</v>
       </c>
       <c r="B579">
@@ -67343,7 +67341,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -67815,7 +67813,7 @@
     </row>
     <row r="21" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>43472</v>
+        <v>43107</v>
       </c>
       <c r="B21">
         <v>74.400000000000006</v>
@@ -67882,17 +67880,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="25">
+    <row r="24" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>43113</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="26">
         <v>75</v>
       </c>
-      <c r="G24" s="26">
-        <v>1</v>
-      </c>
-      <c r="R24" s="26">
+      <c r="G24" s="25">
+        <v>1</v>
+      </c>
+      <c r="R24" s="25">
         <v>3</v>
       </c>
     </row>
@@ -68288,17 +68286,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="25">
+    <row r="44" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>43148</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="26">
         <v>74</v>
       </c>
-      <c r="G44" s="26">
-        <v>1</v>
-      </c>
-      <c r="R44" s="26">
+      <c r="G44" s="25">
+        <v>1</v>
+      </c>
+      <c r="R44" s="25">
         <v>3</v>
       </c>
     </row>
@@ -68362,17 +68360,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="25">
+    <row r="48" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
         <v>43155</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="26">
         <v>73.8</v>
       </c>
-      <c r="G48" s="26">
-        <v>1</v>
-      </c>
-      <c r="R48" s="26">
+      <c r="G48" s="25">
+        <v>1</v>
+      </c>
+      <c r="R48" s="25">
         <v>3</v>
       </c>
     </row>
@@ -68396,17 +68394,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="25">
+    <row r="50" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
         <v>43158</v>
       </c>
-      <c r="B50" s="27">
+      <c r="B50" s="26">
         <v>72.8</v>
       </c>
-      <c r="Q50" s="26">
-        <v>1</v>
-      </c>
-      <c r="R50" s="26">
+      <c r="Q50" s="25">
+        <v>1</v>
+      </c>
+      <c r="R50" s="25">
         <v>2</v>
       </c>
     </row>
@@ -68464,7 +68462,7 @@
     </row>
     <row r="53" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>39512</v>
+        <v>43164</v>
       </c>
       <c r="B53" s="9">
         <v>73.8</v>
@@ -68536,14 +68534,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="25">
+    <row r="57" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
         <v>43172</v>
       </c>
-      <c r="B57" s="27">
+      <c r="B57" s="26">
         <v>72.400000000000006</v>
       </c>
-      <c r="C57" s="26">
+      <c r="C57" s="25">
         <v>1</v>
       </c>
     </row>
@@ -68641,7 +68639,7 @@
     </row>
     <row r="62" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>42816</v>
+        <v>43181</v>
       </c>
       <c r="B62" s="9">
         <v>74</v>
@@ -68699,20 +68697,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="25">
+    <row r="65" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
         <v>43186</v>
       </c>
-      <c r="B65" s="27">
+      <c r="B65" s="26">
         <v>73.8</v>
       </c>
-      <c r="C65" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="26">
-        <v>1</v>
-      </c>
-      <c r="R65" s="26">
+      <c r="C65" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="25">
+        <v>1</v>
+      </c>
+      <c r="R65" s="25">
         <v>3</v>
       </c>
     </row>
@@ -68905,14 +68903,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A75" s="25">
-        <v>43935</v>
-      </c>
-      <c r="B75" s="27">
+    <row r="75" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B75" s="26">
         <v>74.8</v>
       </c>
-      <c r="G75" s="26">
+      <c r="G75" s="25">
         <v>1</v>
       </c>
     </row>
@@ -69219,23 +69217,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="25">
+    <row r="91" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
         <v>43232</v>
       </c>
-      <c r="B91" s="27">
+      <c r="B91" s="26">
         <v>75.400000000000006</v>
       </c>
-      <c r="G91" s="26">
-        <v>1</v>
-      </c>
-      <c r="O91" s="26">
-        <v>1</v>
-      </c>
-      <c r="R91" s="26">
-        <v>3</v>
-      </c>
-      <c r="S91" s="26" t="s">
+      <c r="G91" s="25">
+        <v>1</v>
+      </c>
+      <c r="O91" s="25">
+        <v>1</v>
+      </c>
+      <c r="R91" s="25">
+        <v>3</v>
+      </c>
+      <c r="S91" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -69775,23 +69773,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A117" s="25">
+    <row r="117" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
         <v>43277</v>
       </c>
-      <c r="B117" s="27">
+      <c r="B117" s="26">
         <v>76.599999999999994</v>
       </c>
-      <c r="C117" s="26">
-        <v>1</v>
-      </c>
-      <c r="G117" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q117" s="26">
-        <v>1</v>
-      </c>
-      <c r="R117" s="26">
+      <c r="C117" s="25">
+        <v>1</v>
+      </c>
+      <c r="G117" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q117" s="25">
+        <v>1</v>
+      </c>
+      <c r="R117" s="25">
         <v>2</v>
       </c>
     </row>
@@ -69907,17 +69905,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A123" s="25">
+    <row r="123" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
         <v>43288</v>
       </c>
-      <c r="B123" s="27">
+      <c r="B123" s="26">
         <v>77.2</v>
       </c>
-      <c r="G123" s="26">
-        <v>1</v>
-      </c>
-      <c r="R123" s="26">
+      <c r="G123" s="25">
+        <v>1</v>
+      </c>
+      <c r="R123" s="25">
         <v>3</v>
       </c>
     </row>
@@ -70021,34 +70019,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A129" s="25">
+    <row r="129" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A129" s="3">
         <v>43298</v>
       </c>
-      <c r="B129" s="27">
+      <c r="B129" s="26">
         <v>78.400000000000006</v>
       </c>
-      <c r="C129" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q129" s="26">
-        <v>1</v>
-      </c>
-      <c r="R129" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A130" s="25">
+      <c r="C129" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q129" s="25">
+        <v>1</v>
+      </c>
+      <c r="R129" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A130" s="3">
         <v>43300</v>
       </c>
-      <c r="B130" s="27">
+      <c r="B130" s="26">
         <v>78.400000000000006</v>
       </c>
-      <c r="Q130" s="26">
-        <v>1</v>
-      </c>
-      <c r="R130" s="26">
+      <c r="Q130" s="25">
+        <v>1</v>
+      </c>
+      <c r="R130" s="25">
         <v>3</v>
       </c>
     </row>
@@ -70109,26 +70107,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:19" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A134" s="25">
+    <row r="134" spans="1:19" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A134" s="3">
         <v>43307</v>
       </c>
-      <c r="B134" s="27">
+      <c r="B134" s="26">
         <v>78.599999999999994</v>
       </c>
-      <c r="D134" s="26">
-        <v>1</v>
-      </c>
-      <c r="E134" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q134" s="26">
-        <v>1</v>
-      </c>
-      <c r="R134" s="26">
-        <v>2</v>
-      </c>
-      <c r="S134" s="26" t="s">
+      <c r="D134" s="25">
+        <v>1</v>
+      </c>
+      <c r="E134" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q134" s="25">
+        <v>1</v>
+      </c>
+      <c r="R134" s="25">
+        <v>2</v>
+      </c>
+      <c r="S134" s="25" t="s">
         <v>16</v>
       </c>
     </row>
@@ -70738,7 +70736,7 @@
     </row>
     <row r="164" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
-        <v>43724</v>
+        <v>43359</v>
       </c>
       <c r="B164" s="9">
         <v>76.2</v>
@@ -70756,20 +70754,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A165" s="25">
+    <row r="165" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A165" s="3">
         <v>43361</v>
       </c>
-      <c r="B165" s="27">
+      <c r="B165" s="26">
         <v>76</v>
       </c>
-      <c r="C165" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q165" s="26">
-        <v>1</v>
-      </c>
-      <c r="R165" s="26">
+      <c r="C165" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q165" s="25">
+        <v>1</v>
+      </c>
+      <c r="R165" s="25">
         <v>3</v>
       </c>
     </row>
@@ -70971,17 +70969,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A175" s="25">
+    <row r="175" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A175" s="3">
         <v>43379</v>
       </c>
-      <c r="B175" s="27">
+      <c r="B175" s="26">
         <v>75.8</v>
       </c>
-      <c r="G175" s="26">
-        <v>1</v>
-      </c>
-      <c r="R175" s="26">
+      <c r="G175" s="25">
+        <v>1</v>
+      </c>
+      <c r="R175" s="25">
         <v>3</v>
       </c>
     </row>
@@ -71251,7 +71249,7 @@
     </row>
     <row r="188" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
-        <v>43766</v>
+        <v>43401</v>
       </c>
       <c r="B188" s="9">
         <v>74.8</v>
@@ -71414,7 +71412,7 @@
     </row>
     <row r="196" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
-        <v>43780</v>
+        <v>43415</v>
       </c>
       <c r="B196" s="9">
         <v>73.599999999999994</v>
@@ -71552,20 +71550,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A203" s="25">
+    <row r="203" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A203" s="3">
         <v>43429</v>
       </c>
-      <c r="B203" s="27">
+      <c r="B203" s="26">
         <v>73.8</v>
       </c>
-      <c r="F203" s="26">
-        <v>1</v>
-      </c>
-      <c r="H203" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q203" s="26">
+      <c r="F203" s="25">
+        <v>1</v>
+      </c>
+      <c r="H203" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q203" s="25">
         <v>1</v>
       </c>
     </row>
@@ -71732,20 +71730,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A212" s="25">
+    <row r="212" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A212" s="3">
         <v>43445</v>
       </c>
-      <c r="B212" s="27">
+      <c r="B212" s="26">
         <v>73.8</v>
       </c>
-      <c r="C212" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q212" s="26">
-        <v>1</v>
-      </c>
-      <c r="R212" s="26">
+      <c r="C212" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q212" s="25">
+        <v>1</v>
+      </c>
+      <c r="R212" s="25">
         <v>4</v>
       </c>
     </row>
@@ -71998,20 +71996,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A225" s="25">
+    <row r="225" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A225" s="3">
         <v>43470</v>
       </c>
-      <c r="B225" s="27">
+      <c r="B225" s="26">
         <v>73.599999999999994</v>
       </c>
-      <c r="D225" s="26">
-        <v>1</v>
-      </c>
-      <c r="E225" s="26">
-        <v>1</v>
-      </c>
-      <c r="R225" s="26">
+      <c r="D225" s="25">
+        <v>1</v>
+      </c>
+      <c r="E225" s="25">
+        <v>1</v>
+      </c>
+      <c r="R225" s="25">
         <v>6</v>
       </c>
     </row>
@@ -72748,17 +72746,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A261" s="25">
+    <row r="261" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A261" s="3">
         <v>43533</v>
       </c>
-      <c r="B261" s="27">
+      <c r="B261" s="26">
         <v>73.8</v>
       </c>
-      <c r="G261" s="26">
-        <v>1</v>
-      </c>
-      <c r="R261" s="26">
+      <c r="G261" s="25">
+        <v>1</v>
+      </c>
+      <c r="R261" s="25">
         <v>3</v>
       </c>
     </row>
@@ -72908,17 +72906,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A269" s="25">
+    <row r="269" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A269" s="3">
         <v>43547</v>
       </c>
-      <c r="B269" s="27">
+      <c r="B269" s="26">
         <v>73.599999999999994</v>
       </c>
-      <c r="G269" s="26">
-        <v>1</v>
-      </c>
-      <c r="R269" s="26">
+      <c r="G269" s="25">
+        <v>1</v>
+      </c>
+      <c r="R269" s="25">
         <v>3</v>
       </c>
     </row>
@@ -72994,14 +72992,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A273" s="25">
+    <row r="273" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A273" s="3">
         <v>43554</v>
       </c>
-      <c r="B273" s="27">
+      <c r="B273" s="26">
         <v>73.8</v>
       </c>
-      <c r="G273" s="26">
+      <c r="G273" s="25">
         <v>1</v>
       </c>
     </row>
@@ -73151,17 +73149,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A281" s="25">
+    <row r="281" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A281" s="3">
         <v>43568</v>
       </c>
-      <c r="B281" s="27">
+      <c r="B281" s="26">
         <v>73.8</v>
       </c>
-      <c r="G281" s="26">
-        <v>1</v>
-      </c>
-      <c r="R281" s="26">
+      <c r="G281" s="25">
+        <v>1</v>
+      </c>
+      <c r="R281" s="25">
         <v>3</v>
       </c>
     </row>
@@ -73231,14 +73229,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A285" s="25">
-        <v>43210</v>
-      </c>
-      <c r="B285" s="27">
+    <row r="285" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A285" s="3">
+        <v>43575</v>
+      </c>
+      <c r="B285" s="26">
         <v>73.8</v>
       </c>
-      <c r="G285" s="26">
+      <c r="G285" s="25">
         <v>1</v>
       </c>
     </row>
@@ -73305,11 +73303,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A289" s="25">
+    <row r="289" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A289" s="3">
         <v>43582</v>
       </c>
-      <c r="B289" s="27">
+      <c r="B289" s="26">
         <v>73.8</v>
       </c>
     </row>
@@ -73382,17 +73380,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A293" s="25">
+    <row r="293" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A293" s="3">
         <v>43589</v>
       </c>
-      <c r="B293" s="27">
+      <c r="B293" s="26">
         <v>73</v>
       </c>
-      <c r="G293" s="26">
-        <v>1</v>
-      </c>
-      <c r="R293" s="26">
+      <c r="G293" s="25">
+        <v>1</v>
+      </c>
+      <c r="R293" s="25">
         <v>2</v>
       </c>
     </row>
@@ -73681,7 +73679,7 @@
     </row>
     <row r="308" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A308" s="5">
-        <v>43981</v>
+        <v>43615</v>
       </c>
       <c r="B308" s="9">
         <v>74.2</v>
@@ -73710,7 +73708,7 @@
     </row>
     <row r="309" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A309" s="5">
-        <v>43983</v>
+        <v>43617</v>
       </c>
       <c r="B309" s="9">
         <v>74.599999999999994</v>
@@ -73724,7 +73722,7 @@
     </row>
     <row r="310" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
-        <v>43984</v>
+        <v>43618</v>
       </c>
       <c r="B310" s="9">
         <v>74.599999999999994</v>
@@ -73744,7 +73742,7 @@
     </row>
     <row r="311" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A311" s="5">
-        <v>43986</v>
+        <v>43620</v>
       </c>
       <c r="B311" s="9">
         <v>74.8</v>
@@ -73767,7 +73765,7 @@
     </row>
     <row r="312" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A312" s="5">
-        <v>43988</v>
+        <v>43622</v>
       </c>
       <c r="B312" s="9">
         <v>74.400000000000006</v>
@@ -73793,7 +73791,7 @@
     </row>
     <row r="313" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A313" s="5">
-        <v>43990</v>
+        <v>43624</v>
       </c>
       <c r="B313" s="9">
         <v>74.400000000000006</v>
@@ -73807,7 +73805,7 @@
     </row>
     <row r="314" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
-        <v>43991</v>
+        <v>43625</v>
       </c>
       <c r="B314" s="9">
         <v>74.2</v>
@@ -73821,7 +73819,7 @@
     </row>
     <row r="315" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A315" s="5">
-        <v>43993</v>
+        <v>43627</v>
       </c>
       <c r="B315" s="9">
         <v>74.599999999999994</v>
@@ -73844,7 +73842,7 @@
     </row>
     <row r="316" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A316" s="5">
-        <v>43995</v>
+        <v>43629</v>
       </c>
       <c r="B316" s="9">
         <v>74.599999999999994</v>
@@ -73871,23 +73869,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="28">
-        <v>43997</v>
-      </c>
-      <c r="B317" s="27">
+    <row r="317" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="5">
+        <v>43631</v>
+      </c>
+      <c r="B317" s="26">
         <v>75.599999999999994</v>
       </c>
-      <c r="G317" s="26">
-        <v>1</v>
-      </c>
-      <c r="R317" s="26">
+      <c r="G317" s="25">
+        <v>1</v>
+      </c>
+      <c r="R317" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="318" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
-        <v>43998</v>
+        <v>43632</v>
       </c>
       <c r="B318" s="9">
         <v>75</v>
@@ -73904,7 +73902,7 @@
     </row>
     <row r="319" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A319" s="5">
-        <v>44000</v>
+        <v>43634</v>
       </c>
       <c r="B319" s="9">
         <v>75.599999999999994</v>
@@ -73927,7 +73925,7 @@
     </row>
     <row r="320" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A320" s="5">
-        <v>44002</v>
+        <v>43636</v>
       </c>
       <c r="B320" s="9">
         <v>75.2</v>
@@ -73953,7 +73951,7 @@
     </row>
     <row r="321" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A321" s="5">
-        <v>44004</v>
+        <v>43638</v>
       </c>
       <c r="B321" s="9">
         <v>74.8</v>
@@ -73965,26 +73963,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="28">
-        <v>44005</v>
-      </c>
-      <c r="B322" s="27">
+    <row r="322" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A322" s="5">
+        <v>43639</v>
+      </c>
+      <c r="B322" s="26">
         <v>74.2</v>
       </c>
-      <c r="F322" s="26">
-        <v>1</v>
-      </c>
-      <c r="H322" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q322" s="26">
+      <c r="F322" s="25">
+        <v>1</v>
+      </c>
+      <c r="H322" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q322" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A323" s="5">
-        <v>44007</v>
+        <v>43641</v>
       </c>
       <c r="B323" s="9">
         <v>74.8</v>
@@ -74007,7 +74005,7 @@
     </row>
     <row r="324" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
-        <v>44009</v>
+        <v>43643</v>
       </c>
       <c r="B324" s="9">
         <v>74.8</v>
@@ -74033,7 +74031,7 @@
     </row>
     <row r="325" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A325" s="5">
-        <v>44011</v>
+        <v>43645</v>
       </c>
       <c r="B325" s="9">
         <v>75.2</v>
@@ -74047,7 +74045,7 @@
     </row>
     <row r="326" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A326" s="5">
-        <v>44012</v>
+        <v>43646</v>
       </c>
       <c r="B326" s="9">
         <v>75.2</v>
@@ -74067,7 +74065,7 @@
     </row>
     <row r="327" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A327" s="5">
-        <v>44014</v>
+        <v>43648</v>
       </c>
       <c r="B327" s="9">
         <v>76.2</v>
@@ -74090,7 +74088,7 @@
     </row>
     <row r="328" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
-        <v>44016</v>
+        <v>43650</v>
       </c>
       <c r="B328" s="9">
         <v>75</v>
@@ -74116,7 +74114,7 @@
     </row>
     <row r="329" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
-        <v>44018</v>
+        <v>43652</v>
       </c>
       <c r="B329" s="9">
         <v>75.400000000000006</v>
@@ -74130,7 +74128,7 @@
     </row>
     <row r="330" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A330" s="5">
-        <v>43989</v>
+        <v>43653</v>
       </c>
       <c r="B330" s="9">
         <v>75.400000000000006</v>
@@ -74150,7 +74148,7 @@
     </row>
     <row r="331" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
-        <v>43991</v>
+        <v>43655</v>
       </c>
       <c r="B331" s="9">
         <v>75.8</v>
@@ -74173,7 +74171,7 @@
     </row>
     <row r="332" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
-        <v>44023</v>
+        <v>43657</v>
       </c>
       <c r="B332" s="9">
         <v>74.2</v>
@@ -74202,7 +74200,7 @@
     </row>
     <row r="333" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A333" s="5">
-        <v>44025</v>
+        <v>43659</v>
       </c>
       <c r="B333" s="9">
         <v>74.599999999999994</v>
@@ -74216,7 +74214,7 @@
     </row>
     <row r="334" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A334" s="5">
-        <v>44026</v>
+        <v>43660</v>
       </c>
       <c r="B334" s="9">
         <v>76</v>
@@ -74236,7 +74234,7 @@
     </row>
     <row r="335" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A335" s="5">
-        <v>44028</v>
+        <v>43662</v>
       </c>
       <c r="B335" s="9">
         <v>75.8</v>
@@ -74259,7 +74257,7 @@
     </row>
     <row r="336" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A336" s="5">
-        <v>44030</v>
+        <v>43664</v>
       </c>
       <c r="B336" s="9">
         <v>76</v>
@@ -74285,7 +74283,7 @@
     </row>
     <row r="337" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
-        <v>44032</v>
+        <v>43666</v>
       </c>
       <c r="B337" s="9">
         <v>75.599999999999994</v>
@@ -74299,7 +74297,7 @@
     </row>
     <row r="338" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
-        <v>44033</v>
+        <v>43667</v>
       </c>
       <c r="B338" s="9">
         <v>76</v>
@@ -74319,7 +74317,7 @@
     </row>
     <row r="339" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
-        <v>44035</v>
+        <v>43669</v>
       </c>
       <c r="B339" s="9">
         <v>75.8</v>
@@ -74336,7 +74334,7 @@
     </row>
     <row r="340" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
-        <v>44037</v>
+        <v>43671</v>
       </c>
       <c r="B340" s="9">
         <v>76</v>
@@ -74356,7 +74354,7 @@
     </row>
     <row r="341" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
-        <v>44039</v>
+        <v>43673</v>
       </c>
       <c r="B341" s="9">
         <v>76.599999999999994</v>
@@ -74370,7 +74368,7 @@
     </row>
     <row r="342" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
-        <v>44040</v>
+        <v>43674</v>
       </c>
       <c r="B342" s="9">
         <v>76.2</v>
@@ -74390,7 +74388,7 @@
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
-        <v>44042</v>
+        <v>43676</v>
       </c>
       <c r="B343" s="9">
         <v>76.599999999999994</v>
@@ -74413,7 +74411,7 @@
     </row>
     <row r="344" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
-        <v>44044</v>
+        <v>43678</v>
       </c>
       <c r="B344" s="9">
         <v>76.599999999999994</v>
@@ -74436,7 +74434,7 @@
     </row>
     <row r="345" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A345" s="5">
-        <v>44046</v>
+        <v>43680</v>
       </c>
       <c r="B345" s="9">
         <v>76.8</v>
@@ -74450,7 +74448,7 @@
     </row>
     <row r="346" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A346" s="5">
-        <v>44047</v>
+        <v>43681</v>
       </c>
       <c r="B346" s="9">
         <v>77.8</v>
@@ -74470,7 +74468,7 @@
     </row>
     <row r="347" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A347" s="5">
-        <v>44049</v>
+        <v>43683</v>
       </c>
       <c r="B347" s="9">
         <v>76.8</v>
@@ -74493,7 +74491,7 @@
     </row>
     <row r="348" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A348" s="5">
-        <v>44051</v>
+        <v>43685</v>
       </c>
       <c r="B348" s="9">
         <v>77</v>
@@ -74516,7 +74514,7 @@
     </row>
     <row r="349" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A349" s="5">
-        <v>44053</v>
+        <v>43687</v>
       </c>
       <c r="B349" s="9">
         <v>77.2</v>
@@ -74533,7 +74531,7 @@
     </row>
     <row r="350" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A350" s="5">
-        <v>44054</v>
+        <v>43688</v>
       </c>
       <c r="B350" s="9">
         <v>77.400000000000006</v>
@@ -74553,7 +74551,7 @@
     </row>
     <row r="351" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A351" s="5">
-        <v>44056</v>
+        <v>43690</v>
       </c>
       <c r="B351" s="9">
         <v>76.599999999999994</v>
@@ -74576,7 +74574,7 @@
     </row>
     <row r="352" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A352" s="5">
-        <v>44058</v>
+        <v>43692</v>
       </c>
       <c r="B352" s="9">
         <v>76.2</v>
@@ -74605,7 +74603,7 @@
     </row>
     <row r="353" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A353" s="5">
-        <v>44060</v>
+        <v>43694</v>
       </c>
       <c r="B353" s="9">
         <v>76.599999999999994</v>
@@ -74617,23 +74615,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A354" s="28">
-        <v>44061</v>
-      </c>
-      <c r="B354" s="27">
+    <row r="354" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="5">
+        <v>43695</v>
+      </c>
+      <c r="B354" s="26">
         <v>76.2</v>
       </c>
-      <c r="F354" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q354" s="26">
+      <c r="F354" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q354" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="355" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A355" s="5">
-        <v>44063</v>
+        <v>43697</v>
       </c>
       <c r="B355" s="9">
         <v>76.2</v>
@@ -74659,7 +74657,7 @@
     </row>
     <row r="356" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A356" s="5">
-        <v>44065</v>
+        <v>43699</v>
       </c>
       <c r="B356" s="9">
         <v>75.8</v>
@@ -74679,7 +74677,7 @@
     </row>
     <row r="357" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A357" s="5">
-        <v>44067</v>
+        <v>43701</v>
       </c>
       <c r="B357" s="9">
         <v>76</v>
@@ -74693,7 +74691,7 @@
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A358" s="5">
-        <v>44068</v>
+        <v>43702</v>
       </c>
       <c r="B358" s="9">
         <v>76.400000000000006</v>
@@ -74713,7 +74711,7 @@
     </row>
     <row r="359" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A359" s="5">
-        <v>44070</v>
+        <v>43704</v>
       </c>
       <c r="B359" s="9">
         <v>75.400000000000006</v>
@@ -74736,7 +74734,7 @@
     </row>
     <row r="360" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A360" s="5">
-        <v>44072</v>
+        <v>43706</v>
       </c>
       <c r="B360" s="9">
         <v>76.2</v>
@@ -74762,7 +74760,7 @@
     </row>
     <row r="361" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A361" s="5">
-        <v>44074</v>
+        <v>43708</v>
       </c>
       <c r="B361" s="9">
         <v>76.2</v>
@@ -74776,7 +74774,7 @@
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A362" s="5">
-        <v>44075</v>
+        <v>43709</v>
       </c>
       <c r="B362" s="9">
         <v>75</v>
@@ -74793,7 +74791,7 @@
     </row>
     <row r="363" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A363" s="5">
-        <v>44077</v>
+        <v>43711</v>
       </c>
       <c r="B363" s="9">
         <v>75.400000000000006</v>
@@ -74817,32 +74815,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A364" s="28">
-        <v>44079</v>
-      </c>
-      <c r="B364" s="27">
+    <row r="364" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="5">
+        <v>43713</v>
+      </c>
+      <c r="B364" s="26">
         <v>75.8</v>
       </c>
-      <c r="D364" s="26">
-        <v>1</v>
-      </c>
-      <c r="E364" s="26">
-        <v>1</v>
-      </c>
-      <c r="L364" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q364" s="26">
-        <v>1</v>
-      </c>
-      <c r="R364" s="26">
+      <c r="D364" s="25">
+        <v>1</v>
+      </c>
+      <c r="E364" s="25">
+        <v>1</v>
+      </c>
+      <c r="L364" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q364" s="25">
+        <v>1</v>
+      </c>
+      <c r="R364" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="365" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A365" s="5">
-        <v>44081</v>
+        <v>43715</v>
       </c>
       <c r="B365" s="9">
         <v>75.8</v>
@@ -74859,7 +74857,7 @@
     </row>
     <row r="366" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A366" s="5">
-        <v>44082</v>
+        <v>43716</v>
       </c>
       <c r="B366" s="9">
         <v>77</v>
@@ -74877,29 +74875,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A367" s="28">
-        <v>44084</v>
-      </c>
-      <c r="B367" s="27">
+    <row r="367" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="5">
+        <v>43718</v>
+      </c>
+      <c r="B367" s="26">
         <v>75.599999999999994</v>
       </c>
-      <c r="C367" s="26">
-        <v>1</v>
-      </c>
-      <c r="K367" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q367" s="26">
-        <v>2</v>
-      </c>
-      <c r="R367" s="26">
+      <c r="C367" s="25">
+        <v>1</v>
+      </c>
+      <c r="K367" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q367" s="25">
+        <v>2</v>
+      </c>
+      <c r="R367" s="25">
         <v>4</v>
       </c>
     </row>
     <row r="368" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A368" s="5">
-        <v>44086</v>
+        <v>43720</v>
       </c>
       <c r="B368" s="9">
         <v>75.599999999999994</v>
@@ -74928,7 +74926,7 @@
     </row>
     <row r="369" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A369" s="5">
-        <v>44088</v>
+        <v>43722</v>
       </c>
       <c r="B369" s="9">
         <v>75.599999999999994</v>
@@ -74945,7 +74943,7 @@
     </row>
     <row r="370" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A370" s="5">
-        <v>44089</v>
+        <v>43723</v>
       </c>
       <c r="B370" s="9">
         <v>75.400000000000006</v>
@@ -74965,7 +74963,7 @@
     </row>
     <row r="371" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A371" s="5">
-        <v>44091</v>
+        <v>43725</v>
       </c>
       <c r="B371" s="9">
         <v>75.2</v>
@@ -74991,7 +74989,7 @@
     </row>
     <row r="372" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A372" s="5">
-        <v>44092</v>
+        <v>43726</v>
       </c>
       <c r="B372" s="9">
         <v>75</v>
@@ -75017,7 +75015,7 @@
     </row>
     <row r="373" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A373" s="5">
-        <v>44095</v>
+        <v>43729</v>
       </c>
       <c r="B373" s="9">
         <v>75</v>
@@ -75034,7 +75032,7 @@
     </row>
     <row r="374" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A374" s="5">
-        <v>44096</v>
+        <v>43730</v>
       </c>
       <c r="B374" s="9">
         <v>74.400000000000006</v>
@@ -75051,7 +75049,7 @@
     </row>
     <row r="375" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A375" s="5">
-        <v>44098</v>
+        <v>43732</v>
       </c>
       <c r="B375" s="9">
         <v>74.599999999999994</v>
@@ -75074,7 +75072,7 @@
     </row>
     <row r="376" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A376" s="5">
-        <v>44100</v>
+        <v>43734</v>
       </c>
       <c r="B376" s="9">
         <v>74.400000000000006</v>
@@ -75100,7 +75098,7 @@
     </row>
     <row r="377" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A377" s="5">
-        <v>44102</v>
+        <v>43736</v>
       </c>
       <c r="B377" s="9">
         <v>74.599999999999994</v>
@@ -75114,7 +75112,7 @@
     </row>
     <row r="378" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A378" s="5">
-        <v>44103</v>
+        <v>43737</v>
       </c>
       <c r="B378" s="9">
         <v>74.400000000000006</v>
@@ -75134,7 +75132,7 @@
     </row>
     <row r="379" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A379" s="5">
-        <v>44105</v>
+        <v>43739</v>
       </c>
       <c r="B379">
         <v>73.8</v>
@@ -75160,7 +75158,7 @@
     </row>
     <row r="380" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A380" s="5">
-        <v>44107</v>
+        <v>43741</v>
       </c>
       <c r="B380">
         <v>73.400000000000006</v>
@@ -75184,23 +75182,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="381" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A381" s="28">
-        <v>44109</v>
-      </c>
-      <c r="B381" s="26">
+    <row r="381" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="5">
+        <v>43743</v>
+      </c>
+      <c r="B381" s="25">
         <v>73.8</v>
       </c>
-      <c r="G381" s="26">
-        <v>1</v>
-      </c>
-      <c r="R381" s="26">
+      <c r="G381" s="25">
+        <v>1</v>
+      </c>
+      <c r="R381" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="382" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A382" s="5">
-        <v>44110</v>
+        <v>43744</v>
       </c>
       <c r="B382">
         <v>73.599999999999994</v>
@@ -75220,7 +75218,7 @@
     </row>
     <row r="383" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
-        <v>44112</v>
+        <v>43746</v>
       </c>
       <c r="B383">
         <v>73.2</v>
@@ -75246,7 +75244,7 @@
     </row>
     <row r="384" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A384" s="5">
-        <v>44114</v>
+        <v>43748</v>
       </c>
       <c r="B384">
         <v>73</v>
@@ -75272,7 +75270,7 @@
     </row>
     <row r="385" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A385" s="5">
-        <v>44116</v>
+        <v>43750</v>
       </c>
       <c r="B385">
         <v>73.400000000000006</v>
@@ -75286,7 +75284,7 @@
     </row>
     <row r="386" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A386" s="5">
-        <v>44117</v>
+        <v>43751</v>
       </c>
       <c r="B386">
         <v>73</v>
@@ -75306,7 +75304,7 @@
     </row>
     <row r="387" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A387" s="5">
-        <v>44119</v>
+        <v>43753</v>
       </c>
       <c r="B387">
         <v>77.2</v>
@@ -75332,7 +75330,7 @@
     </row>
     <row r="388" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A388" s="5">
-        <v>44121</v>
+        <v>43755</v>
       </c>
       <c r="B388">
         <v>72</v>
@@ -75358,7 +75356,7 @@
     </row>
     <row r="389" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A389" s="5">
-        <v>44123</v>
+        <v>43757</v>
       </c>
       <c r="B389">
         <v>73</v>
@@ -75372,7 +75370,7 @@
     </row>
     <row r="390" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A390" s="5">
-        <v>44124</v>
+        <v>43758</v>
       </c>
       <c r="B390">
         <v>72.8</v>
@@ -75392,7 +75390,7 @@
     </row>
     <row r="391" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A391" s="5">
-        <v>44126</v>
+        <v>43760</v>
       </c>
       <c r="B391">
         <v>73</v>
@@ -75418,7 +75416,7 @@
     </row>
     <row r="392" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A392" s="5">
-        <v>44128</v>
+        <v>43762</v>
       </c>
       <c r="B392">
         <v>73.400000000000006</v>
@@ -75444,7 +75442,7 @@
     </row>
     <row r="393" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A393" s="5">
-        <v>44130</v>
+        <v>43764</v>
       </c>
       <c r="B393">
         <v>72.8</v>
@@ -75458,7 +75456,7 @@
     </row>
     <row r="394" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A394" s="5">
-        <v>44132</v>
+        <v>43766</v>
       </c>
       <c r="B394">
         <v>73</v>
@@ -75478,7 +75476,7 @@
     </row>
     <row r="395" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A395" s="5">
-        <v>44133</v>
+        <v>43767</v>
       </c>
       <c r="B395">
         <v>73</v>
@@ -75504,7 +75502,7 @@
     </row>
     <row r="396" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A396" s="5">
-        <v>44135</v>
+        <v>43769</v>
       </c>
       <c r="B396">
         <v>72.400000000000006</v>
@@ -75530,7 +75528,7 @@
     </row>
     <row r="397" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A397" s="5">
-        <v>44137</v>
+        <v>43771</v>
       </c>
       <c r="B397">
         <v>72.8</v>
@@ -75544,7 +75542,7 @@
     </row>
     <row r="398" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A398" s="5">
-        <v>44138</v>
+        <v>43772</v>
       </c>
       <c r="B398">
         <v>73</v>
@@ -75564,7 +75562,7 @@
     </row>
     <row r="399" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A399" s="5">
-        <v>44140</v>
+        <v>43774</v>
       </c>
       <c r="B399">
         <v>73.2</v>
@@ -75590,7 +75588,7 @@
     </row>
     <row r="400" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A400" s="5">
-        <v>44142</v>
+        <v>43776</v>
       </c>
       <c r="B400">
         <v>72.599999999999994</v>
@@ -75613,7 +75611,7 @@
     </row>
     <row r="401" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A401" s="5">
-        <v>44144</v>
+        <v>43778</v>
       </c>
       <c r="B401">
         <v>72.8</v>
@@ -75625,26 +75623,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A402" s="28">
-        <v>44145</v>
-      </c>
-      <c r="B402" s="26">
+    <row r="402" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A402" s="5">
+        <v>43779</v>
+      </c>
+      <c r="B402" s="25">
         <v>72.8</v>
       </c>
-      <c r="F402" s="26">
-        <v>1</v>
-      </c>
-      <c r="H402" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q402" s="26">
+      <c r="F402" s="25">
+        <v>1</v>
+      </c>
+      <c r="H402" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q402" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A403" s="5">
-        <v>44147</v>
+        <v>43781</v>
       </c>
       <c r="B403">
         <v>73.400000000000006</v>
@@ -75664,7 +75662,7 @@
     </row>
     <row r="404" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
-        <v>44149</v>
+        <v>43783</v>
       </c>
       <c r="B404">
         <v>73</v>
@@ -75690,7 +75688,7 @@
     </row>
     <row r="405" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A405" s="5">
-        <v>44151</v>
+        <v>43785</v>
       </c>
       <c r="B405">
         <v>73</v>
@@ -75704,7 +75702,7 @@
     </row>
     <row r="406" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A406" s="5">
-        <v>44152</v>
+        <v>43786</v>
       </c>
       <c r="B406">
         <v>72.8</v>
@@ -75724,7 +75722,7 @@
     </row>
     <row r="407" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A407" s="5">
-        <v>44154</v>
+        <v>43788</v>
       </c>
       <c r="B407">
         <v>73.599999999999994</v>
@@ -75748,46 +75746,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="408" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="28">
-        <v>44156</v>
-      </c>
-      <c r="B408" s="26">
+    <row r="408" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A408" s="5">
+        <v>43790</v>
+      </c>
+      <c r="B408" s="25">
         <v>73.599999999999994</v>
       </c>
-      <c r="D408" s="26">
-        <v>1</v>
-      </c>
-      <c r="E408" s="26">
-        <v>1</v>
-      </c>
-      <c r="M408" s="26">
-        <v>1</v>
-      </c>
-      <c r="N408" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q408" s="26">
-        <v>3</v>
-      </c>
-      <c r="R408" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="409" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="28">
-        <v>44158</v>
-      </c>
-      <c r="B409" s="26">
+      <c r="D408" s="25">
+        <v>1</v>
+      </c>
+      <c r="E408" s="25">
+        <v>1</v>
+      </c>
+      <c r="M408" s="25">
+        <v>1</v>
+      </c>
+      <c r="N408" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q408" s="25">
+        <v>3</v>
+      </c>
+      <c r="R408" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A409" s="5">
+        <v>43792</v>
+      </c>
+      <c r="B409" s="25">
         <v>73.8</v>
       </c>
-      <c r="G409" s="26">
+      <c r="G409" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="410" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A410" s="5">
-        <v>44159</v>
+        <v>43793</v>
       </c>
       <c r="B410">
         <v>73.400000000000006</v>
@@ -75807,7 +75805,7 @@
     </row>
     <row r="411" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A411" s="5">
-        <v>44161</v>
+        <v>43795</v>
       </c>
       <c r="B411">
         <v>73.599999999999994</v>
@@ -75833,7 +75831,7 @@
     </row>
     <row r="412" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A412" s="5">
-        <v>44165</v>
+        <v>43799</v>
       </c>
       <c r="B412">
         <v>72.599999999999994</v>
@@ -75847,7 +75845,7 @@
     </row>
     <row r="413" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A413" s="5">
-        <v>44166</v>
+        <v>43800</v>
       </c>
       <c r="B413" s="9">
         <v>72.8</v>
@@ -75867,7 +75865,7 @@
     </row>
     <row r="414" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A414" s="5">
-        <v>44168</v>
+        <v>43802</v>
       </c>
       <c r="B414" s="9">
         <v>73.2</v>
@@ -75893,7 +75891,7 @@
     </row>
     <row r="415" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A415" s="5">
-        <v>44170</v>
+        <v>43804</v>
       </c>
       <c r="B415" s="9">
         <v>73.8</v>
@@ -75919,7 +75917,7 @@
     </row>
     <row r="416" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A416" s="5">
-        <v>44172</v>
+        <v>43806</v>
       </c>
       <c r="B416" s="9">
         <v>73.400000000000006</v>
@@ -75933,7 +75931,7 @@
     </row>
     <row r="417" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A417" s="5">
-        <v>44173</v>
+        <v>43807</v>
       </c>
       <c r="B417" s="9">
         <v>73.8</v>
@@ -75953,7 +75951,7 @@
     </row>
     <row r="418" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A418" s="5">
-        <v>44175</v>
+        <v>43809</v>
       </c>
       <c r="B418" s="9">
         <v>74</v>
@@ -75979,7 +75977,7 @@
     </row>
     <row r="419" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A419" s="5">
-        <v>44177</v>
+        <v>43811</v>
       </c>
       <c r="B419" s="9">
         <v>74.2</v>
@@ -76003,23 +76001,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="420" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A420" s="28">
-        <v>44180</v>
-      </c>
-      <c r="B420" s="27">
+    <row r="420" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A420" s="5">
+        <v>43814</v>
+      </c>
+      <c r="B420" s="26">
         <v>74.2</v>
       </c>
-      <c r="F420" s="26">
-        <v>1</v>
-      </c>
-      <c r="H420" s="26">
+      <c r="F420" s="25">
+        <v>1</v>
+      </c>
+      <c r="H420" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="421" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
-        <v>44181</v>
+        <v>43815</v>
       </c>
       <c r="B421" s="9">
         <v>74</v>
@@ -76039,7 +76037,7 @@
     </row>
     <row r="422" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A422" s="5">
-        <v>44182</v>
+        <v>43816</v>
       </c>
       <c r="B422" s="9">
         <v>73.8</v>
@@ -76065,7 +76063,7 @@
     </row>
     <row r="423" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A423" s="5">
-        <v>44184</v>
+        <v>43818</v>
       </c>
       <c r="B423" s="9">
         <v>73.599999999999994</v>
@@ -76082,7 +76080,7 @@
     </row>
     <row r="424" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A424" s="5">
-        <v>44186</v>
+        <v>43820</v>
       </c>
       <c r="B424" s="9">
         <v>73</v>
@@ -76096,7 +76094,7 @@
     </row>
     <row r="425" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A425" s="5">
-        <v>44187</v>
+        <v>43821</v>
       </c>
       <c r="B425" s="9">
         <v>73.599999999999994</v>
@@ -76116,7 +76114,7 @@
     </row>
     <row r="426" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A426" s="5">
-        <v>44189</v>
+        <v>43823</v>
       </c>
       <c r="B426" s="9">
         <v>73.400000000000006</v>
@@ -76140,43 +76138,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A427" s="28">
-        <v>44191</v>
-      </c>
-      <c r="B427" s="27">
+    <row r="427" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A427" s="5">
+        <v>43825</v>
+      </c>
+      <c r="B427" s="26">
         <v>73.599999999999994</v>
       </c>
-      <c r="D427" s="26">
-        <v>1</v>
-      </c>
-      <c r="E427" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q427" s="26">
-        <v>1</v>
-      </c>
-      <c r="R427" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="428" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A428" s="28">
-        <v>44193</v>
-      </c>
-      <c r="B428" s="27">
+      <c r="D427" s="25">
+        <v>1</v>
+      </c>
+      <c r="E427" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q427" s="25">
+        <v>1</v>
+      </c>
+      <c r="R427" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="428" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A428" s="5">
+        <v>43827</v>
+      </c>
+      <c r="B428" s="26">
         <v>73</v>
       </c>
-      <c r="G428" s="26">
-        <v>1</v>
-      </c>
-      <c r="R428" s="26">
+      <c r="G428" s="25">
+        <v>1</v>
+      </c>
+      <c r="R428" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="429" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A429" s="5">
-        <v>44194</v>
+        <v>43828</v>
       </c>
       <c r="B429" s="9">
         <v>73.599999999999994</v>
@@ -76196,7 +76194,7 @@
     </row>
     <row r="430" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A430" s="5">
-        <v>44196</v>
+        <v>43830</v>
       </c>
       <c r="B430" s="9">
         <v>73.400000000000006</v>
@@ -76435,40 +76433,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="441" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A441" s="28">
+    <row r="441" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A441" s="5">
         <v>43849</v>
       </c>
-      <c r="B441" s="27">
+      <c r="B441" s="26">
         <v>73.2</v>
       </c>
-      <c r="C441" s="26">
-        <v>1</v>
-      </c>
-      <c r="F441" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q441" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="442" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A442" s="28">
+      <c r="C441" s="25">
+        <v>1</v>
+      </c>
+      <c r="F441" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q441" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A442" s="5">
         <v>43851</v>
       </c>
-      <c r="B442" s="27">
+      <c r="B442" s="26">
         <v>73</v>
       </c>
-      <c r="C442" s="26">
-        <v>1</v>
-      </c>
-      <c r="K442" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q442" s="26">
-        <v>1</v>
-      </c>
-      <c r="R442" s="26">
+      <c r="C442" s="25">
+        <v>1</v>
+      </c>
+      <c r="K442" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q442" s="25">
+        <v>1</v>
+      </c>
+      <c r="R442" s="25">
         <v>3</v>
       </c>
     </row>
@@ -76839,17 +76837,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="460" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A460" s="28">
+    <row r="460" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A460" s="5">
         <v>43883</v>
       </c>
-      <c r="B460" s="27">
+      <c r="B460" s="26">
         <v>73</v>
       </c>
-      <c r="G460" s="26">
-        <v>1</v>
-      </c>
-      <c r="R460" s="26">
+      <c r="G460" s="25">
+        <v>1</v>
+      </c>
+      <c r="R460" s="25">
         <v>2</v>
       </c>
     </row>
@@ -77160,54 +77158,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A475" s="28">
+    <row r="475" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A475" s="5">
         <v>43909</v>
       </c>
-      <c r="B475" s="27">
+      <c r="B475" s="26">
         <v>74.599999999999994</v>
       </c>
-      <c r="D475" s="26">
-        <v>1</v>
-      </c>
-      <c r="E475" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q475" s="26">
-        <v>4</v>
-      </c>
-      <c r="R475" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="476" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A476" s="28">
+      <c r="D475" s="25">
+        <v>1</v>
+      </c>
+      <c r="E475" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q475" s="25">
+        <v>4</v>
+      </c>
+      <c r="R475" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="476" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A476" s="5">
         <v>43911</v>
       </c>
-      <c r="B476" s="27">
+      <c r="B476" s="26">
         <v>74.400000000000006</v>
       </c>
-      <c r="F476" s="26">
-        <v>1</v>
-      </c>
-      <c r="R476" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="477" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A477" s="28">
+      <c r="F476" s="25">
+        <v>1</v>
+      </c>
+      <c r="R476" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="477" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A477" s="5">
         <v>43912</v>
       </c>
-      <c r="B477" s="27">
+      <c r="B477" s="26">
         <v>74.599999999999994</v>
       </c>
-      <c r="F477" s="26">
-        <v>1</v>
-      </c>
-      <c r="H477" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q477" s="26">
+      <c r="F477" s="25">
+        <v>1</v>
+      </c>
+      <c r="H477" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q477" s="25">
         <v>4</v>
       </c>
     </row>
@@ -77397,14 +77395,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="487" spans="1:18" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A487" s="25">
+    <row r="487" spans="1:18" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A487" s="3">
         <v>43932</v>
       </c>
-      <c r="B487" s="27">
+      <c r="B487" s="26">
         <v>73.8</v>
       </c>
-      <c r="G487" s="26">
+      <c r="G487" s="25">
         <v>1</v>
       </c>
     </row>
@@ -78687,7 +78685,7 @@
     </row>
     <row r="549" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A549" s="22">
-        <v>44045</v>
+        <v>44044</v>
       </c>
       <c r="B549" s="9">
         <v>77.2</v>
@@ -78702,7 +78700,7 @@
     </row>
     <row r="550" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A550" s="22">
-        <v>44046</v>
+        <v>44045</v>
       </c>
       <c r="B550" s="9">
         <v>77</v>
@@ -79276,7 +79274,7 @@
       </c>
     </row>
     <row r="578" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A578" s="30">
+      <c r="A578" s="28">
         <v>44094</v>
       </c>
       <c r="B578" s="9">
@@ -79463,34 +79461,34 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="35" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">

</xml_diff>

<commit_message>
Tried to do VAR regression, but I am having problems with getting it to work because of our NA's
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/753f33f7ae04b4eb/Documents/Fall 2020/Stat 495R/final-project-danny_brady_michael/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{69618D21-8C0B-44B8-9C0B-1BAB8B51074F}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAC705F9-0A17-40E8-B0D6-E17949026D9E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces Eaten" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
   <si>
     <t>Pieces Eaten</t>
   </si>
@@ -893,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
@@ -67339,9 +67339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S592"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -67800,9 +67800,6 @@
       </c>
       <c r="G20">
         <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>41</v>
       </c>
       <c r="J20">
         <v>1</v>

</xml_diff>

<commit_message>
Did some more work on VAR
</commit_message>
<xml_diff>
--- a/SharkData.xlsx
+++ b/SharkData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/753f33f7ae04b4eb/Documents/Fall 2020/Stat 495R/final-project-danny_brady_michael/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAC705F9-0A17-40E8-B0D6-E17949026D9E}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_BEF785862E17B9DF8A3E8FDDBB77C52D50B09033" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4CED88E-8231-4002-BEC1-72698706C511}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces Eaten" sheetId="1" r:id="rId1"/>
@@ -345,28 +345,33 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -894,8 +899,8 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C511" sqref="C511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4160,7 +4165,7 @@
         <v>0</v>
       </c>
       <c r="N83" s="7">
-        <f t="shared" ref="N83:N241" si="1">SUM(B83:M83)</f>
+        <f t="shared" ref="N83:N242" si="1">SUM(B83:M83)</f>
         <v>23</v>
       </c>
     </row>
@@ -10343,6 +10348,10 @@
       </c>
       <c r="M242" s="1">
         <v>0</v>
+      </c>
+      <c r="N242" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="243" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -25125,8 +25134,8 @@
   <dimension ref="A1:O593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A584"/>
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -46217,8 +46226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O593"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:A584"/>
     </sheetView>
   </sheetViews>
@@ -67339,7 +67348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S592"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>

</xml_diff>